<commit_message>
Added age breakdown per suburb
</commit_message>
<xml_diff>
--- a/ProjectedPopulationGrowth.xlsx
+++ b/ProjectedPopulationGrowth.xlsx
@@ -9,13 +9,14 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="1170" yWindow="0" windowWidth="27630" windowHeight="13290"/>
+    <workbookView xWindow="2340" yWindow="0" windowWidth="27630" windowHeight="13290"/>
   </bookViews>
   <sheets>
     <sheet name="PopulationGrowth" sheetId="1" r:id="rId1"/>
-    <sheet name="HighProjections" sheetId="4" r:id="rId2"/>
-    <sheet name="MediumProjections" sheetId="5" r:id="rId3"/>
-    <sheet name="LowProjections" sheetId="6" r:id="rId4"/>
+    <sheet name="StatisticalAreaDPTIProjections" sheetId="7" r:id="rId2"/>
+    <sheet name="HighProjections" sheetId="4" r:id="rId3"/>
+    <sheet name="MediumProjections" sheetId="5" r:id="rId4"/>
+    <sheet name="LowProjections" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="171027"/>
   <extLst>
@@ -27,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="874" uniqueCount="66">
   <si>
     <t>Projected population growth per suburb</t>
   </si>
@@ -193,6 +194,39 @@
   <si>
     <t>2030 vs 2015</t>
   </si>
+  <si>
+    <t>Statistical area</t>
+  </si>
+  <si>
+    <t>Playford (C) - Elizabeth</t>
+  </si>
+  <si>
+    <t>Walkerville (M)</t>
+  </si>
+  <si>
+    <t>Charles Sturt (C) - North-East</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0-4  </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total </t>
+  </si>
+  <si>
+    <t>Statistical Local Area (SLA)</t>
+  </si>
+  <si>
+    <t>Sex</t>
+  </si>
+  <si>
+    <t>Year</t>
+  </si>
+  <si>
+    <t>Age ranges</t>
+  </si>
+  <si>
+    <t>Growth</t>
+  </si>
 </sst>
 </file>
 
@@ -243,7 +277,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="20">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -254,23 +288,11 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
@@ -291,6 +313,23 @@
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -605,7 +644,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AA22"/>
+  <dimension ref="A1:AB22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection sqref="A1:H1"/>
@@ -617,183 +656,188 @@
     <col min="2" max="2" width="21.7109375" style="1" bestFit="1" customWidth="1"/>
     <col min="3" max="14" width="9.140625" style="1"/>
     <col min="15" max="15" width="20.5703125" style="1" bestFit="1" customWidth="1"/>
-    <col min="16" max="16384" width="9.140625" style="1"/>
+    <col min="16" max="16" width="9.140625" style="1"/>
+    <col min="17" max="17" width="26.85546875" style="4" bestFit="1" customWidth="1"/>
+    <col min="18" max="16384" width="9.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:27" ht="23.25" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:28" ht="23.25" x14ac:dyDescent="0.25">
+      <c r="A1" s="15" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
-      <c r="D1" s="4"/>
-      <c r="E1" s="4"/>
-      <c r="F1" s="4"/>
-      <c r="G1" s="4"/>
-      <c r="H1" s="4"/>
+      <c r="B1" s="15"/>
+      <c r="C1" s="15"/>
+      <c r="D1" s="15"/>
+      <c r="E1" s="15"/>
+      <c r="F1" s="15"/>
+      <c r="G1" s="15"/>
+      <c r="H1" s="15"/>
       <c r="I1" s="3"/>
       <c r="J1" s="3"/>
       <c r="K1" s="3"/>
       <c r="L1" s="3"/>
       <c r="M1" s="3"/>
     </row>
-    <row r="2" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+    <row r="2" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A2" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="7"/>
-      <c r="C2" s="7"/>
-      <c r="D2" s="7"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-      <c r="G2" s="7"/>
-      <c r="H2" s="7"/>
-      <c r="I2" s="8"/>
-      <c r="J2" s="8"/>
-      <c r="K2" s="8"/>
-      <c r="L2" s="8"/>
-      <c r="M2" s="8"/>
-    </row>
-    <row r="3" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A3" s="5" t="s">
+      <c r="B2" s="14"/>
+      <c r="C2" s="14"/>
+      <c r="D2" s="14"/>
+      <c r="E2" s="14"/>
+      <c r="F2" s="14"/>
+      <c r="G2" s="14"/>
+      <c r="H2" s="14"/>
+      <c r="I2" s="5"/>
+      <c r="J2" s="5"/>
+      <c r="K2" s="5"/>
+      <c r="L2" s="5"/>
+      <c r="M2" s="5"/>
+    </row>
+    <row r="3" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A3" s="17" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="5"/>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-    </row>
-    <row r="4" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A4" s="6" t="s">
+      <c r="B3" s="17"/>
+      <c r="C3" s="17"/>
+      <c r="D3" s="17"/>
+      <c r="E3" s="17"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="17"/>
+      <c r="H3" s="17"/>
+    </row>
+    <row r="4" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A4" s="16" t="s">
         <v>1</v>
       </c>
-      <c r="B4" s="6"/>
-      <c r="C4" s="6"/>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="6"/>
+      <c r="B4" s="16"/>
+      <c r="C4" s="16"/>
+      <c r="D4" s="16"/>
+      <c r="E4" s="16"/>
+      <c r="F4" s="16"/>
+      <c r="G4" s="16"/>
+      <c r="H4" s="16"/>
       <c r="I4" s="2"/>
       <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
       <c r="M4" s="2"/>
     </row>
-    <row r="6" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+    <row r="6" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A6" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="B6" s="7"/>
-      <c r="C6" s="14"/>
-      <c r="D6" s="14"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="10" t="s">
+      <c r="B6" s="14"/>
+      <c r="C6" s="10"/>
+      <c r="D6" s="10"/>
+      <c r="E6" s="10"/>
+      <c r="F6" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G6" s="10"/>
-      <c r="H6" s="10"/>
-      <c r="I6" s="10" t="s">
+      <c r="G6" s="13"/>
+      <c r="H6" s="13"/>
+      <c r="I6" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J6" s="10"/>
-      <c r="K6" s="10"/>
-      <c r="L6" s="10" t="s">
+      <c r="J6" s="13"/>
+      <c r="K6" s="13"/>
+      <c r="L6" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M6" s="10"/>
-      <c r="N6" s="10"/>
-      <c r="O6" s="9" t="s">
+      <c r="M6" s="13"/>
+      <c r="N6" s="13"/>
+      <c r="O6" s="6" t="s">
         <v>53</v>
       </c>
-      <c r="Q6" s="8" t="s">
+      <c r="Q6" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="R6" s="5" t="s">
         <v>52</v>
       </c>
-      <c r="W6" s="8" t="s">
+      <c r="X6" s="5" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="7" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A7" s="8" t="s">
+    <row r="7" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A7" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B7" s="8" t="s">
+      <c r="B7" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C7" s="8">
+      <c r="C7" s="5">
         <v>2006</v>
       </c>
-      <c r="D7" s="8">
+      <c r="D7" s="5">
         <v>2011</v>
       </c>
-      <c r="E7" s="8">
+      <c r="E7" s="5">
         <v>2015</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="5">
         <v>2020</v>
       </c>
-      <c r="G7" s="8">
+      <c r="G7" s="5">
         <v>2025</v>
       </c>
-      <c r="H7" s="8">
+      <c r="H7" s="5">
         <v>2030</v>
       </c>
-      <c r="I7" s="8">
+      <c r="I7" s="5">
         <v>2020</v>
       </c>
-      <c r="J7" s="8">
+      <c r="J7" s="5">
         <v>2025</v>
       </c>
-      <c r="K7" s="8">
+      <c r="K7" s="5">
         <v>2030</v>
       </c>
-      <c r="L7" s="8">
+      <c r="L7" s="5">
         <v>2020</v>
       </c>
-      <c r="M7" s="8">
+      <c r="M7" s="5">
         <v>2025</v>
       </c>
-      <c r="N7" s="8">
+      <c r="N7" s="5">
         <v>2030</v>
       </c>
-      <c r="O7" s="8" t="s">
+      <c r="O7" s="5" t="s">
         <v>54</v>
       </c>
-      <c r="Q7" s="8">
+      <c r="R7" s="5">
         <v>2011</v>
       </c>
-      <c r="R7" s="8">
+      <c r="S7" s="5">
         <v>2015</v>
       </c>
-      <c r="S7" s="8">
+      <c r="T7" s="5">
         <v>2020</v>
       </c>
-      <c r="T7" s="8">
+      <c r="U7" s="5">
         <v>2025</v>
       </c>
-      <c r="U7" s="8">
+      <c r="V7" s="5">
         <v>2030</v>
       </c>
-      <c r="W7" s="8">
+      <c r="X7" s="5">
         <v>2011</v>
       </c>
-      <c r="X7" s="8">
+      <c r="Y7" s="5">
         <v>2015</v>
       </c>
-      <c r="Y7" s="8">
+      <c r="Z7" s="5">
         <v>2020</v>
       </c>
-      <c r="Z7" s="8">
+      <c r="AA7" s="5">
         <v>2025</v>
       </c>
-      <c r="AA7" s="8">
+      <c r="AB7" s="5">
         <v>2030</v>
       </c>
     </row>
-    <row r="8" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A8" s="1">
         <v>5112</v>
       </c>
@@ -809,78 +853,81 @@
       <c r="E8" s="1">
         <v>18739</v>
       </c>
-      <c r="F8" s="15">
-        <f>E8*(1 + $Y$8*LowProjections!N$27)</f>
+      <c r="F8" s="11">
+        <f>E8*(1 + $Z$8*LowProjections!N$27)</f>
         <v>18982.024064272173</v>
       </c>
-      <c r="G8" s="15">
-        <f>F8*(1 + $Z$8*LowProjections!O$27)</f>
+      <c r="G8" s="11">
+        <f>F8*(1 + $AA$8*LowProjections!O$27)</f>
         <v>19148.126766046702</v>
       </c>
-      <c r="H8" s="15">
-        <f>G8*(1 + $AA$8*LowProjections!P$27)</f>
+      <c r="H8" s="11">
+        <f>G8*(1 + $AB$8*LowProjections!P$27)</f>
         <v>19228.642036766552</v>
       </c>
-      <c r="I8" s="15">
-        <f>E8*(1 + $Y$8*MediumProjections!N$27)</f>
+      <c r="I8" s="11">
+        <f>E8*(1 + $Z$8*MediumProjections!N$27)</f>
         <v>19068.866180411987</v>
       </c>
-      <c r="J8" s="15">
-        <f>I8*(1 + $Z$8*MediumProjections!O$27)</f>
+      <c r="J8" s="11">
+        <f>I8*(1 + $AA$8*MediumProjections!O$27)</f>
         <v>19381.226169670099</v>
       </c>
-      <c r="K8" s="15">
-        <f>J8*(1 + $AA$8*MediumProjections!P$27)</f>
+      <c r="K8" s="11">
+        <f>J8*(1 + $AB$8*MediumProjections!P$27)</f>
         <v>19545.116926312683</v>
       </c>
-      <c r="L8" s="15">
-        <f>E8*(1 + $Y$8*HighProjections!N$27)</f>
+      <c r="L8" s="11">
+        <f>E8*(1 + $Z$8*HighProjections!N$27)</f>
         <v>18986.654552207394</v>
       </c>
-      <c r="M8" s="15">
-        <f>L8*(1 + $Z$8*HighProjections!O$27)</f>
+      <c r="M8" s="11">
+        <f>L8*(1 + $AA$8*HighProjections!O$27)</f>
         <v>19225.685777402945</v>
       </c>
-      <c r="N8" s="15">
-        <f>M8*(1 + $AA$8*HighProjections!P$27)</f>
+      <c r="N8" s="11">
+        <f>M8*(1 + $AB$8*HighProjections!P$27)</f>
         <v>19364.844535729619</v>
       </c>
-      <c r="O8" s="16">
+      <c r="O8" s="12">
         <f>(K8/E8)-1</f>
         <v>4.3018140045503195E-2</v>
       </c>
-      <c r="Q8" s="13">
+      <c r="Q8" s="4" t="s">
+        <v>56</v>
+      </c>
+      <c r="R8" s="9">
         <v>0</v>
       </c>
-      <c r="R8" s="13">
+      <c r="S8" s="9">
         <v>2.7379704066177402E-2</v>
       </c>
-      <c r="S8" s="13">
+      <c r="T8" s="9">
         <v>1.9921372949270433E-2</v>
       </c>
-      <c r="T8" s="13">
+      <c r="U8" s="9">
         <v>1.7086097624254171E-2</v>
       </c>
-      <c r="U8" s="13">
+      <c r="V8" s="9">
         <v>8.4541943007070408E-3</v>
       </c>
-      <c r="W8" s="12">
+      <c r="X8" s="8">
         <v>0</v>
       </c>
-      <c r="X8" s="12">
+      <c r="Y8" s="8">
         <v>0.50058700492192743</v>
       </c>
-      <c r="Y8" s="12">
+      <c r="Z8" s="8">
         <v>0.3712103898026814</v>
       </c>
-      <c r="Z8" s="12">
+      <c r="AA8" s="8">
         <v>0.36246255275217293</v>
       </c>
-      <c r="AA8" s="12">
+      <c r="AB8" s="8">
         <v>0.20790917206649251</v>
       </c>
     </row>
-    <row r="9" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>5011</v>
       </c>
@@ -896,78 +943,81 @@
       <c r="E9" s="1">
         <v>9729</v>
       </c>
-      <c r="F9" s="15">
-        <f>E9*(1 + $Y$9*LowProjections!N$27)</f>
+      <c r="F9" s="11">
+        <f>E9*(1 + $Z$9*LowProjections!N$27)</f>
         <v>10278.921275921623</v>
       </c>
-      <c r="G9" s="15">
-        <f>F9*(1 + $Z$9*LowProjections!O$27)</f>
+      <c r="G9" s="11">
+        <f>F9*(1 + $AA$9*LowProjections!O$27)</f>
         <v>10657.607033671411</v>
       </c>
-      <c r="H9" s="15">
-        <f>G9*(1 + $AA$9*LowProjections!P$27)</f>
+      <c r="H9" s="11">
+        <f>G9*(1 + $AB$9*LowProjections!P$27)</f>
         <v>10906.441648648544</v>
       </c>
-      <c r="I9" s="15">
-        <f>E9*(1 + $Y$9*MediumProjections!N$27)</f>
+      <c r="I9" s="11">
+        <f>E9*(1 + $Z$9*MediumProjections!N$27)</f>
         <v>10475.429911617284</v>
       </c>
-      <c r="J9" s="15">
-        <f>I9*(1 + $Z$9*MediumProjections!O$27)</f>
+      <c r="J9" s="11">
+        <f>I9*(1 + $AA$9*MediumProjections!O$27)</f>
         <v>11197.86634276823</v>
       </c>
-      <c r="K9" s="15">
-        <f>J9*(1 + $AA$9*MediumProjections!P$27)</f>
+      <c r="K9" s="11">
+        <f>J9*(1 + $AB$9*MediumProjections!P$27)</f>
         <v>11723.650647639699</v>
       </c>
-      <c r="L9" s="15">
-        <f>E9*(1 + $Y$9*HighProjections!N$27)</f>
+      <c r="L9" s="11">
+        <f>E9*(1 + $Z$9*HighProjections!N$27)</f>
         <v>10289.399266408296</v>
       </c>
-      <c r="M9" s="15">
-        <f>L9*(1 + $Z$9*HighProjections!O$27)</f>
+      <c r="M9" s="11">
+        <f>L9*(1 + $AA$9*HighProjections!O$27)</f>
         <v>10834.772052958575</v>
       </c>
-      <c r="N9" s="15">
-        <f>M9*(1 + $AA$9*HighProjections!P$27)</f>
+      <c r="N9" s="11">
+        <f>M9*(1 + $AB$9*HighProjections!P$27)</f>
         <v>11270.231394600012</v>
       </c>
-      <c r="O9" s="16">
+      <c r="O9" s="12">
         <f t="shared" ref="O9:O10" si="0">(K9/E9)-1</f>
         <v>0.20502113759273288</v>
       </c>
-      <c r="Q9" s="13">
+      <c r="Q9" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="R9" s="9">
         <v>0</v>
       </c>
-      <c r="R9" s="13">
+      <c r="S9" s="9">
         <v>0.11848374439461873</v>
       </c>
-      <c r="S9" s="13">
+      <c r="T9" s="9">
         <v>8.6825784626949787E-2</v>
       </c>
-      <c r="T9" s="13">
+      <c r="U9" s="9">
         <v>7.1934981843333912E-2</v>
       </c>
-      <c r="U9" s="13">
+      <c r="V9" s="9">
         <v>4.6943055331505112E-2</v>
       </c>
-      <c r="W9" s="12">
+      <c r="X9" s="8">
         <v>0</v>
       </c>
-      <c r="X9" s="12">
+      <c r="Y9" s="8">
         <v>2.1662550696340714</v>
       </c>
-      <c r="Y9" s="12">
+      <c r="Z9" s="8">
         <v>1.6178921723100441</v>
       </c>
-      <c r="Z9" s="12">
+      <c r="AA9" s="8">
         <v>1.5260206118747475</v>
       </c>
-      <c r="AA9" s="12">
+      <c r="AB9" s="8">
         <v>1.1544437495869402</v>
       </c>
     </row>
-    <row r="10" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>5081</v>
       </c>
@@ -983,150 +1033,153 @@
       <c r="E10" s="1">
         <v>8694</v>
       </c>
-      <c r="F10" s="15">
-        <f>E10*(1 + $Y$10*LowProjections!N$27)</f>
+      <c r="F10" s="11">
+        <f>E10*(1 + $Z$10*LowProjections!N$27)</f>
         <v>8717.0919137665278</v>
       </c>
-      <c r="G10" s="15">
-        <f>F10*(1 + $Z$10*LowProjections!O$27)</f>
+      <c r="G10" s="11">
+        <f>F10*(1 + $AA$10*LowProjections!O$27)</f>
         <v>8735.8371856641388</v>
       </c>
-      <c r="H10" s="15">
-        <f>G10*(1 + $AA$10*LowProjections!P$27)</f>
+      <c r="H10" s="11">
+        <f>G10*(1 + $AB$10*LowProjections!P$27)</f>
         <v>8741.6976454234718</v>
       </c>
-      <c r="I10" s="15">
-        <f>E10*(1 + $Y$10*MediumProjections!N$27)</f>
+      <c r="I10" s="11">
+        <f>E10*(1 + $Z$10*MediumProjections!N$27)</f>
         <v>8725.3435684461128</v>
       </c>
-      <c r="J10" s="15">
-        <f>I10*(1 + $Z$10*MediumProjections!O$27)</f>
+      <c r="J10" s="11">
+        <f>I10*(1 + $AA$10*MediumProjections!O$27)</f>
         <v>8760.4671671747019</v>
       </c>
-      <c r="K10" s="15">
-        <f>J10*(1 + $AA$10*MediumProjections!P$27)</f>
+      <c r="K10" s="11">
+        <f>J10*(1 + $AB$10*MediumProjections!P$27)</f>
         <v>8772.2860294097718</v>
       </c>
-      <c r="L10" s="15">
-        <f>E10*(1 + $Y$10*HighProjections!N$27)</f>
+      <c r="L10" s="11">
+        <f>E10*(1 + $Z$10*HighProjections!N$27)</f>
         <v>8717.5318982940571</v>
       </c>
-      <c r="M10" s="15">
-        <f>L10*(1 + $Z$10*HighProjections!O$27)</f>
+      <c r="M10" s="11">
+        <f>L10*(1 + $AA$10*HighProjections!O$27)</f>
         <v>8744.5021919957981</v>
       </c>
-      <c r="N10" s="15">
-        <f>M10*(1 + $AA$10*HighProjections!P$27)</f>
+      <c r="N10" s="11">
+        <f>M10*(1 + $AB$10*HighProjections!P$27)</f>
         <v>8754.6002762374119</v>
       </c>
-      <c r="O10" s="16">
+      <c r="O10" s="12">
         <f t="shared" si="0"/>
         <v>9.0046042569325024E-3</v>
       </c>
-      <c r="Q10" s="13">
+      <c r="Q10" s="4" t="s">
+        <v>57</v>
+      </c>
+      <c r="R10" s="9">
         <v>0</v>
       </c>
-      <c r="R10" s="13">
+      <c r="S10" s="9">
         <v>6.1576354679802048E-3</v>
       </c>
-      <c r="S10" s="13">
+      <c r="T10" s="9">
         <v>4.0799673602611719E-3</v>
       </c>
-      <c r="T10" s="13">
+      <c r="U10" s="9">
         <v>4.1988351618582609E-3</v>
       </c>
-      <c r="U10" s="13">
+      <c r="V10" s="9">
         <v>1.3487995683840737E-3</v>
       </c>
-      <c r="W10" s="12">
+      <c r="X10" s="8">
         <v>0</v>
       </c>
-      <c r="X10" s="12">
+      <c r="Y10" s="8">
         <v>0.11258092084804602</v>
       </c>
-      <c r="Y10" s="12">
+      <c r="Z10" s="8">
         <v>7.6025195554618244E-2</v>
       </c>
-      <c r="Z10" s="12">
+      <c r="AA10" s="8">
         <v>8.907361673927941E-2</v>
       </c>
-      <c r="AA10" s="12">
+      <c r="AB10" s="8">
         <v>3.3170257457049747E-2</v>
       </c>
     </row>
-    <row r="12" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A12" s="7" t="s">
+    <row r="12" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A12" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="7"/>
-      <c r="C12" s="14"/>
-      <c r="D12" s="14"/>
-      <c r="E12" s="14"/>
-      <c r="F12" s="10" t="s">
+      <c r="B12" s="14"/>
+      <c r="C12" s="10"/>
+      <c r="D12" s="10"/>
+      <c r="E12" s="10"/>
+      <c r="F12" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G12" s="10"/>
-      <c r="H12" s="10"/>
-      <c r="I12" s="10" t="s">
+      <c r="G12" s="13"/>
+      <c r="H12" s="13"/>
+      <c r="I12" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J12" s="10"/>
-      <c r="K12" s="10"/>
-      <c r="L12" s="10" t="s">
+      <c r="J12" s="13"/>
+      <c r="K12" s="13"/>
+      <c r="L12" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M12" s="10"/>
-      <c r="N12" s="10"/>
-      <c r="O12" s="9"/>
-    </row>
-    <row r="13" spans="1:27" x14ac:dyDescent="0.25">
-      <c r="A13" s="8" t="s">
+      <c r="M12" s="13"/>
+      <c r="N12" s="13"/>
+      <c r="O12" s="6"/>
+    </row>
+    <row r="13" spans="1:28" x14ac:dyDescent="0.25">
+      <c r="A13" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B13" s="8" t="s">
+      <c r="B13" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C13" s="8">
+      <c r="C13" s="5">
         <v>2006</v>
       </c>
-      <c r="D13" s="8">
+      <c r="D13" s="5">
         <v>2011</v>
       </c>
-      <c r="E13" s="8">
+      <c r="E13" s="5">
         <v>2015</v>
       </c>
-      <c r="F13" s="8">
+      <c r="F13" s="5">
         <v>2020</v>
       </c>
-      <c r="G13" s="8">
+      <c r="G13" s="5">
         <v>2025</v>
       </c>
-      <c r="H13" s="8">
+      <c r="H13" s="5">
         <v>2030</v>
       </c>
-      <c r="I13" s="8">
+      <c r="I13" s="5">
         <v>2020</v>
       </c>
-      <c r="J13" s="8">
+      <c r="J13" s="5">
         <v>2025</v>
       </c>
-      <c r="K13" s="8">
+      <c r="K13" s="5">
         <v>2030</v>
       </c>
-      <c r="L13" s="8">
+      <c r="L13" s="5">
         <v>2020</v>
       </c>
-      <c r="M13" s="8">
+      <c r="M13" s="5">
         <v>2025</v>
       </c>
-      <c r="N13" s="8">
+      <c r="N13" s="5">
         <v>2030</v>
       </c>
-      <c r="O13" s="8">
+      <c r="O13" s="5">
         <v>2030</v>
       </c>
     </row>
-    <row r="14" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A14" s="1">
         <v>5112</v>
       </c>
@@ -1142,48 +1195,48 @@
       <c r="E14" s="1">
         <v>9284</v>
       </c>
-      <c r="F14" s="15">
-        <f>E14*(1 + $Y$8*LowProjections!N$54)</f>
+      <c r="F14" s="11">
+        <f>E14*(1 + $Z$8*LowProjections!N$54)</f>
         <v>9409.2191894065181</v>
       </c>
-      <c r="G14" s="15">
-        <f>F14*(1 + $Z$8*LowProjections!O$54)</f>
+      <c r="G14" s="11">
+        <f>F14*(1 + $AA$8*LowProjections!O$54)</f>
         <v>9494.1336974255828</v>
       </c>
-      <c r="H14" s="15">
-        <f>G14*(1 + $AA$8*LowProjections!P$54)</f>
+      <c r="H14" s="11">
+        <f>G14*(1 + $AB$8*LowProjections!P$54)</f>
         <v>9534.9045471677855</v>
       </c>
-      <c r="I14" s="15">
-        <f>E14*(1 + $Y$8*MediumProjections!N$54)</f>
+      <c r="I14" s="11">
+        <f>E14*(1 + $Z$8*MediumProjections!N$54)</f>
         <v>9453.018406140116</v>
       </c>
-      <c r="J14" s="15">
-        <f>I14*(1 + $Z$8*MediumProjections!O$54)</f>
+      <c r="J14" s="11">
+        <f>I14*(1 + $AA$8*MediumProjections!O$54)</f>
         <v>9611.6191644781338</v>
       </c>
-      <c r="K14" s="15">
-        <f>J14*(1 + $AA$8*MediumProjections!P$54)</f>
+      <c r="K14" s="11">
+        <f>J14*(1 + $AB$8*MediumProjections!P$54)</f>
         <v>9694.2891204337375</v>
       </c>
-      <c r="L14" s="15">
-        <f>E14*(1 + $Y$8*HighProjections!N$54)</f>
+      <c r="L14" s="11">
+        <f>E14*(1 + $Z$8*HighProjections!N$54)</f>
         <v>9410.2974073692367</v>
       </c>
-      <c r="M14" s="15">
-        <f>L14*(1 + $Z$8*HighProjections!O$54)</f>
+      <c r="M14" s="11">
+        <f>L14*(1 + $AA$8*HighProjections!O$54)</f>
         <v>9536.765362846485</v>
       </c>
-      <c r="N14" s="15">
-        <f>M14*(1 + $AA$8*HighProjections!P$54)</f>
+      <c r="N14" s="11">
+        <f>M14*(1 + $AB$8*HighProjections!P$54)</f>
         <v>9609.8407283928645</v>
       </c>
-      <c r="O14" s="16">
+      <c r="O14" s="12">
         <f>(K14/E14)-1</f>
         <v>4.4193140934267294E-2</v>
       </c>
     </row>
-    <row r="15" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A15" s="1">
         <v>5011</v>
       </c>
@@ -1199,48 +1252,48 @@
       <c r="E15" s="1">
         <v>4818</v>
       </c>
-      <c r="F15" s="15">
-        <f>E15*(1 + $Y$9*LowProjections!N$54)</f>
+      <c r="F15" s="11">
+        <f>E15*(1 + $Z$9*LowProjections!N$54)</f>
         <v>5101.2252720355864</v>
       </c>
-      <c r="G15" s="15">
-        <f>F15*(1 + $Z$9*LowProjections!O$54)</f>
+      <c r="G15" s="11">
+        <f>F15*(1 + $AA$9*LowProjections!O$54)</f>
         <v>5295.0459326770497</v>
       </c>
-      <c r="H15" s="15">
-        <f>G15*(1 + $AA$9*LowProjections!P$54)</f>
+      <c r="H15" s="11">
+        <f>G15*(1 + $AB$9*LowProjections!P$54)</f>
         <v>5421.3052042478257</v>
       </c>
-      <c r="I15" s="15">
-        <f>E15*(1 + $Y$9*MediumProjections!N$54)</f>
+      <c r="I15" s="11">
+        <f>E15*(1 + $Z$9*MediumProjections!N$54)</f>
         <v>5200.2919177558897</v>
       </c>
-      <c r="J15" s="15">
-        <f>I15*(1 + $Z$9*MediumProjections!O$54)</f>
+      <c r="J15" s="11">
+        <f>I15*(1 + $AA$9*MediumProjections!O$54)</f>
         <v>5567.6247389340215</v>
       </c>
-      <c r="K15" s="15">
-        <f>J15*(1 + $AA$9*MediumProjections!P$54)</f>
+      <c r="K15" s="11">
+        <f>J15*(1 + $AB$9*MediumProjections!P$54)</f>
         <v>5833.5259009232468</v>
       </c>
-      <c r="L15" s="15">
-        <f>E15*(1 + $Y$9*HighProjections!N$54)</f>
+      <c r="L15" s="11">
+        <f>E15*(1 + $Z$9*HighProjections!N$54)</f>
         <v>5103.6640242528174</v>
       </c>
-      <c r="M15" s="15">
-        <f>L15*(1 + $Z$9*HighProjections!O$54)</f>
+      <c r="M15" s="11">
+        <f>L15*(1 + $AA$9*HighProjections!O$54)</f>
         <v>5392.4369547659317</v>
       </c>
-      <c r="N15" s="15">
-        <f>M15*(1 + $AA$9*HighProjections!P$54)</f>
+      <c r="N15" s="11">
+        <f>M15*(1 + $AB$9*HighProjections!P$54)</f>
         <v>5621.8690139085102</v>
       </c>
-      <c r="O15" s="16">
+      <c r="O15" s="12">
         <f t="shared" ref="O15:O16" si="1">(K15/E15)-1</f>
         <v>0.21077748047389933</v>
       </c>
     </row>
-    <row r="16" spans="1:27" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:28" x14ac:dyDescent="0.25">
       <c r="A16" s="1">
         <v>5081</v>
       </c>
@@ -1256,116 +1309,116 @@
       <c r="E16" s="1">
         <v>4193</v>
       </c>
-      <c r="F16" s="15">
-        <f>E16*(1 + $Y$10*LowProjections!N$54)</f>
+      <c r="F16" s="11">
+        <f>E16*(1 + $Z$10*LowProjections!N$54)</f>
         <v>4204.5823861899853</v>
       </c>
-      <c r="G16" s="15">
-        <f>F16*(1 + $Z$10*LowProjections!O$54)</f>
+      <c r="G16" s="11">
+        <f>F16*(1 + $AA$10*LowProjections!O$54)</f>
         <v>4213.9071345507473</v>
       </c>
-      <c r="H16" s="15">
-        <f>G16*(1 + $AA$110*LowProjections!P$54)</f>
+      <c r="H16" s="11">
+        <f>G16*(1 + $AB$110*LowProjections!P$54)</f>
         <v>4213.9071345507473</v>
       </c>
-      <c r="I16" s="15">
-        <f>E16*(1 + $Y$10*MediumProjections!N$54)</f>
+      <c r="I16" s="11">
+        <f>E16*(1 + $Z$10*MediumProjections!N$54)</f>
         <v>4208.6336777326933</v>
       </c>
-      <c r="J16" s="15">
-        <f>I16*(1 + $Z$10*MediumProjections!O$54)</f>
+      <c r="J16" s="11">
+        <f>I16*(1 + $AA$10*MediumProjections!O$54)</f>
         <v>4225.9861685836659</v>
       </c>
-      <c r="K16" s="15">
-        <f>J16*(1 + $AA$10*MediumProjections!P$54)</f>
+      <c r="K16" s="11">
+        <f>J16*(1 + $AB$10*MediumProjections!P$54)</f>
         <v>4231.785186042749</v>
       </c>
-      <c r="L16" s="15">
-        <f>E16*(1 + $Y$10*HighProjections!N$54)</f>
+      <c r="L16" s="11">
+        <f>E16*(1 + $Z$10*HighProjections!N$54)</f>
         <v>4204.6821180034585</v>
       </c>
-      <c r="M16" s="15">
-        <f>L16*(1 + $Z$10*HighProjections!O$54)</f>
+      <c r="M16" s="11">
+        <f>L16*(1 + $AA$10*HighProjections!O$54)</f>
         <v>4218.5687286283755</v>
       </c>
-      <c r="N16" s="15">
-        <f>M16*(1 + $AA$10*HighProjections!P$54)</f>
+      <c r="N16" s="11">
+        <f>M16*(1 + $AB$10*HighProjections!P$54)</f>
         <v>4223.7258840656787</v>
       </c>
-      <c r="O16" s="16">
+      <c r="O16" s="12">
         <f t="shared" si="1"/>
         <v>9.2499847466609442E-3</v>
       </c>
     </row>
     <row r="18" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A18" s="7" t="s">
+      <c r="A18" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="B18" s="7"/>
-      <c r="C18" s="14"/>
-      <c r="D18" s="14"/>
-      <c r="E18" s="14"/>
-      <c r="F18" s="10" t="s">
+      <c r="B18" s="14"/>
+      <c r="C18" s="10"/>
+      <c r="D18" s="10"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="13" t="s">
         <v>49</v>
       </c>
-      <c r="G18" s="10"/>
-      <c r="H18" s="10"/>
-      <c r="I18" s="10" t="s">
+      <c r="G18" s="13"/>
+      <c r="H18" s="13"/>
+      <c r="I18" s="13" t="s">
         <v>50</v>
       </c>
-      <c r="J18" s="10"/>
-      <c r="K18" s="10"/>
-      <c r="L18" s="10" t="s">
+      <c r="J18" s="13"/>
+      <c r="K18" s="13"/>
+      <c r="L18" s="13" t="s">
         <v>51</v>
       </c>
-      <c r="M18" s="10"/>
-      <c r="N18" s="10"/>
-      <c r="O18" s="9"/>
+      <c r="M18" s="13"/>
+      <c r="N18" s="13"/>
+      <c r="O18" s="6"/>
     </row>
     <row r="19" spans="1:15" x14ac:dyDescent="0.25">
-      <c r="A19" s="8" t="s">
+      <c r="A19" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="B19" s="8" t="s">
+      <c r="B19" s="5" t="s">
         <v>6</v>
       </c>
-      <c r="C19" s="8">
+      <c r="C19" s="5">
         <v>2006</v>
       </c>
-      <c r="D19" s="8">
+      <c r="D19" s="5">
         <v>2011</v>
       </c>
-      <c r="E19" s="8">
+      <c r="E19" s="5">
         <v>2015</v>
       </c>
-      <c r="F19" s="8">
+      <c r="F19" s="5">
         <v>2020</v>
       </c>
-      <c r="G19" s="8">
+      <c r="G19" s="5">
         <v>2025</v>
       </c>
-      <c r="H19" s="8">
+      <c r="H19" s="5">
         <v>2030</v>
       </c>
-      <c r="I19" s="8">
+      <c r="I19" s="5">
         <v>2020</v>
       </c>
-      <c r="J19" s="8">
+      <c r="J19" s="5">
         <v>2025</v>
       </c>
-      <c r="K19" s="8">
+      <c r="K19" s="5">
         <v>2030</v>
       </c>
-      <c r="L19" s="8">
+      <c r="L19" s="5">
         <v>2020</v>
       </c>
-      <c r="M19" s="8">
+      <c r="M19" s="5">
         <v>2025</v>
       </c>
-      <c r="N19" s="8">
+      <c r="N19" s="5">
         <v>2030</v>
       </c>
-      <c r="O19" s="8">
+      <c r="O19" s="5">
         <v>2030</v>
       </c>
     </row>
@@ -1385,43 +1438,43 @@
       <c r="E20" s="1">
         <v>9455</v>
       </c>
-      <c r="F20" s="15">
-        <f>E20*(1 + $Y$8*LowProjections!N$81)</f>
+      <c r="F20" s="11">
+        <f>E20*(1 + $Z$8*LowProjections!N$81)</f>
         <v>9572.867769891287</v>
       </c>
-      <c r="G20" s="15">
-        <f>F20*(1 + $Z$8*LowProjections!O$81)</f>
+      <c r="G20" s="11">
+        <f>F20*(1 + $AA$8*LowProjections!O$81)</f>
         <v>9654.0859892726912</v>
       </c>
-      <c r="H20" s="15">
-        <f>G20*(1 + $AA$8*LowProjections!P$81)</f>
+      <c r="H20" s="11">
+        <f>G20*(1 + $AB$8*LowProjections!P$81)</f>
         <v>9693.839735268868</v>
       </c>
-      <c r="I20" s="15">
-        <f>E20*(1 + $Y$8*MediumProjections!N$81)</f>
+      <c r="I20" s="11">
+        <f>E20*(1 + $Z$8*MediumProjections!N$81)</f>
         <v>9615.9204601281472</v>
       </c>
-      <c r="J20" s="15">
-        <f>I20*(1 + $Z$8*MediumProjections!O$81)</f>
+      <c r="J20" s="11">
+        <f>I20*(1 + $AA$8*MediumProjections!O$81)</f>
         <v>9769.7227068760822</v>
       </c>
-      <c r="K20" s="15">
-        <f>J20*(1 + $AA$8*MediumProjections!P$81)</f>
+      <c r="K20" s="11">
+        <f>J20*(1 + $AB$8*MediumProjections!P$81)</f>
         <v>9850.9582126460245</v>
       </c>
-      <c r="L20" s="15">
-        <f>E20*(1 + $Y$8*HighProjections!N$81)</f>
+      <c r="L20" s="11">
+        <f>E20*(1 + $Z$8*HighProjections!N$81)</f>
         <v>9576.3465839151559</v>
       </c>
-      <c r="M20" s="15">
-        <f>L20*(1 + $Z$8*HighProjections!O$81)</f>
+      <c r="M20" s="11">
+        <f>L20*(1 + $AA$8*HighProjections!O$81)</f>
         <v>9688.8762874688273</v>
       </c>
-      <c r="N20" s="15">
-        <f>M20*(1 + $AA$8*HighProjections!P$81)</f>
+      <c r="N20" s="11">
+        <f>M20*(1 + $AB$8*HighProjections!P$81)</f>
         <v>9754.9309097303685</v>
       </c>
-      <c r="O20" s="16">
+      <c r="O20" s="12">
         <f>(K20/E20)-1</f>
         <v>4.1878182194185598E-2</v>
       </c>
@@ -1442,43 +1495,43 @@
       <c r="E21" s="1">
         <v>4911</v>
       </c>
-      <c r="F21" s="15">
-        <f>E21*(1 + $Y$9*LowProjections!N$81)</f>
+      <c r="F21" s="11">
+        <f>E21*(1 + $Z$9*LowProjections!N$81)</f>
         <v>5177.8289321397751</v>
       </c>
-      <c r="G21" s="15">
-        <f>F21*(1 + $Z$9*LowProjections!O$81)</f>
+      <c r="G21" s="11">
+        <f>F21*(1 + $AA$9*LowProjections!O$81)</f>
         <v>5362.7797927707288</v>
       </c>
-      <c r="H21" s="15">
-        <f>G21*(1 + $AA$9*LowProjections!P$81)</f>
+      <c r="H21" s="11">
+        <f>G21*(1 + $AB$9*LowProjections!P$81)</f>
         <v>5485.3982895686831</v>
       </c>
-      <c r="I21" s="15">
-        <f>E21*(1 + $Y$9*MediumProjections!N$81)</f>
+      <c r="I21" s="11">
+        <f>E21*(1 + $Z$9*MediumProjections!N$81)</f>
         <v>5275.2915665159189</v>
       </c>
-      <c r="J21" s="15">
-        <f>I21*(1 + $Z$9*MediumProjections!O$81)</f>
+      <c r="J21" s="11">
+        <f>I21*(1 + $AA$9*MediumProjections!O$81)</f>
         <v>5630.5263961982218</v>
       </c>
-      <c r="K21" s="15">
-        <f>J21*(1 + $AA$9*MediumProjections!P$81)</f>
+      <c r="K21" s="11">
+        <f>J21*(1 + $AB$9*MediumProjections!P$81)</f>
         <v>5890.4895385349591</v>
       </c>
-      <c r="L21" s="15">
-        <f>E21*(1 + $Y$9*HighProjections!N$81)</f>
+      <c r="L21" s="11">
+        <f>E21*(1 + $Z$9*HighProjections!N$81)</f>
         <v>5185.704267627656</v>
       </c>
-      <c r="M21" s="15">
-        <f>L21*(1 + $Z$9*HighProjections!O$81)</f>
+      <c r="M21" s="11">
+        <f>L21*(1 + $AA$9*HighProjections!O$81)</f>
         <v>5442.2544455309926</v>
       </c>
-      <c r="N21" s="15">
-        <f>M21*(1 + $AA$9*HighProjections!P$81)</f>
+      <c r="N21" s="11">
+        <f>M21*(1 + $AB$9*HighProjections!P$81)</f>
         <v>5648.2736819768788</v>
       </c>
-      <c r="O21" s="16">
+      <c r="O21" s="12">
         <f t="shared" ref="O21:O22" si="2">(K21/E21)-1</f>
         <v>0.19944808359498256</v>
       </c>
@@ -1499,49 +1552,58 @@
       <c r="E22" s="1">
         <v>4456</v>
       </c>
-      <c r="F22" s="15">
-        <f>E22*(1 + $Y$10*LowProjections!N$81)</f>
+      <c r="F22" s="11">
+        <f>E22*(1 + $Z$10*LowProjections!N$81)</f>
         <v>4467.3766956062536</v>
       </c>
-      <c r="G22" s="15">
-        <f>F22*(1 + $Z$10*LowProjections!O$81)</f>
+      <c r="G22" s="11">
+        <f>F22*(1 + $AA$10*LowProjections!O$81)</f>
         <v>4476.6909891356408</v>
       </c>
-      <c r="H22" s="15">
-        <f>G22*(1 + $AA$10*LowProjections!P$81)</f>
+      <c r="H22" s="11">
+        <f>G22*(1 + $AB$10*LowProjections!P$81)</f>
         <v>4479.6320174569873</v>
       </c>
-      <c r="I22" s="15">
-        <f>E22*(1 + $Y$10*MediumProjections!N$81)</f>
+      <c r="I22" s="11">
+        <f>E22*(1 + $Z$10*MediumProjections!N$81)</f>
         <v>4471.5321772303387</v>
       </c>
-      <c r="J22" s="15">
-        <f>I22*(1 + $Z$10*MediumProjections!O$81)</f>
+      <c r="J22" s="11">
+        <f>I22*(1 + $AA$10*MediumProjections!O$81)</f>
         <v>4489.1079374747806</v>
       </c>
-      <c r="K22" s="15">
-        <f>J22*(1 + $AA$10*MediumProjections!P$81)</f>
+      <c r="K22" s="11">
+        <f>J22*(1 + $AB$10*MediumProjections!P$81)</f>
         <v>4495.063172320225</v>
       </c>
-      <c r="L22" s="15">
-        <f>E22*(1 + $Y$10*HighProjections!N$81)</f>
+      <c r="L22" s="11">
+        <f>E22*(1 + $Z$10*HighProjections!N$81)</f>
         <v>4467.7124736417318</v>
       </c>
-      <c r="M22" s="15">
-        <f>L22*(1 + $Z$10*HighProjections!O$81)</f>
+      <c r="M22" s="11">
+        <f>L22*(1 + $AA$10*HighProjections!O$81)</f>
         <v>4480.6139222538723</v>
       </c>
-      <c r="N22" s="15">
-        <f>M22*(1 + $AA$10*HighProjections!P$81)</f>
+      <c r="N22" s="11">
+        <f>M22*(1 + $AB$10*HighProjections!P$81)</f>
         <v>4485.4874396442838</v>
       </c>
-      <c r="O22" s="16">
+      <c r="O22" s="12">
         <f t="shared" si="2"/>
         <v>8.7664210772497864E-3</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="16">
+    <mergeCell ref="A1:H1"/>
+    <mergeCell ref="A4:H4"/>
+    <mergeCell ref="A3:H3"/>
+    <mergeCell ref="A2:H2"/>
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A18:B18"/>
+    <mergeCell ref="F6:H6"/>
+    <mergeCell ref="I6:K6"/>
     <mergeCell ref="L6:N6"/>
     <mergeCell ref="F12:H12"/>
     <mergeCell ref="I12:K12"/>
@@ -1549,15 +1611,6 @@
     <mergeCell ref="F18:H18"/>
     <mergeCell ref="I18:K18"/>
     <mergeCell ref="L18:N18"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="A12:B12"/>
-    <mergeCell ref="A18:B18"/>
-    <mergeCell ref="F6:H6"/>
-    <mergeCell ref="I6:K6"/>
-    <mergeCell ref="A1:H1"/>
-    <mergeCell ref="A4:H4"/>
-    <mergeCell ref="A3:H3"/>
-    <mergeCell ref="A2:H2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1565,6 +1618,1642 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:AF21"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="26.85546875" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="9.140625" style="19"/>
+    <col min="29" max="29" width="9.140625" style="19"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A1" s="19" t="s">
+        <v>61</v>
+      </c>
+      <c r="B1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="C1" s="19" t="s">
+        <v>62</v>
+      </c>
+      <c r="D1" s="19" t="s">
+        <v>15</v>
+      </c>
+      <c r="X1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="Y1" s="19" t="s">
+        <v>64</v>
+      </c>
+      <c r="AC1" s="19" t="s">
+        <v>63</v>
+      </c>
+      <c r="AD1" s="19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="D2" s="19" t="s">
+        <v>59</v>
+      </c>
+      <c r="E2" s="19" t="s">
+        <v>24</v>
+      </c>
+      <c r="F2" s="19" t="s">
+        <v>25</v>
+      </c>
+      <c r="G2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="H2" s="19" t="s">
+        <v>27</v>
+      </c>
+      <c r="I2" s="19" t="s">
+        <v>28</v>
+      </c>
+      <c r="J2" s="19" t="s">
+        <v>29</v>
+      </c>
+      <c r="K2" s="19" t="s">
+        <v>30</v>
+      </c>
+      <c r="L2" s="19" t="s">
+        <v>31</v>
+      </c>
+      <c r="M2" s="19" t="s">
+        <v>32</v>
+      </c>
+      <c r="N2" s="19" t="s">
+        <v>33</v>
+      </c>
+      <c r="O2" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="P2" s="19" t="s">
+        <v>35</v>
+      </c>
+      <c r="Q2" s="19" t="s">
+        <v>36</v>
+      </c>
+      <c r="R2" s="19" t="s">
+        <v>37</v>
+      </c>
+      <c r="S2" s="19" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" s="19" t="s">
+        <v>39</v>
+      </c>
+      <c r="U2" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="V2" s="19" t="s">
+        <v>60</v>
+      </c>
+      <c r="W2" s="19"/>
+      <c r="Y2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA2" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB2" s="18"/>
+      <c r="AD2" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE2" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF2" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>58</v>
+      </c>
+      <c r="B3">
+        <v>2010</v>
+      </c>
+      <c r="C3" t="s">
+        <v>22</v>
+      </c>
+      <c r="D3">
+        <v>1748</v>
+      </c>
+      <c r="E3">
+        <v>1534</v>
+      </c>
+      <c r="F3">
+        <v>1554</v>
+      </c>
+      <c r="G3">
+        <v>1782</v>
+      </c>
+      <c r="H3">
+        <v>2240</v>
+      </c>
+      <c r="I3">
+        <v>2386</v>
+      </c>
+      <c r="J3">
+        <v>2076</v>
+      </c>
+      <c r="K3">
+        <v>2118</v>
+      </c>
+      <c r="L3">
+        <v>2202</v>
+      </c>
+      <c r="M3">
+        <v>2010</v>
+      </c>
+      <c r="N3">
+        <v>2031</v>
+      </c>
+      <c r="O3">
+        <v>1592</v>
+      </c>
+      <c r="P3">
+        <v>1267</v>
+      </c>
+      <c r="Q3">
+        <v>898</v>
+      </c>
+      <c r="R3">
+        <v>871</v>
+      </c>
+      <c r="S3">
+        <v>764</v>
+      </c>
+      <c r="T3">
+        <v>693</v>
+      </c>
+      <c r="U3">
+        <v>778</v>
+      </c>
+      <c r="V3">
+        <v>28544</v>
+      </c>
+      <c r="X3" s="19">
+        <v>2010</v>
+      </c>
+      <c r="Y3">
+        <f>SUM(D3:G3)</f>
+        <v>6618</v>
+      </c>
+      <c r="Z3">
+        <f>SUM(H3:Q3)</f>
+        <v>18820</v>
+      </c>
+      <c r="AA3">
+        <f>SUM(R3:U3)</f>
+        <v>3106</v>
+      </c>
+      <c r="AC3" s="19">
+        <v>2010</v>
+      </c>
+      <c r="AD3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE3" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF3" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B4">
+        <v>2015</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+      <c r="D4">
+        <v>2171</v>
+      </c>
+      <c r="E4">
+        <v>1886</v>
+      </c>
+      <c r="F4">
+        <v>1650</v>
+      </c>
+      <c r="G4">
+        <v>1838</v>
+      </c>
+      <c r="H4">
+        <v>2190</v>
+      </c>
+      <c r="I4">
+        <v>2762</v>
+      </c>
+      <c r="J4">
+        <v>2672</v>
+      </c>
+      <c r="K4">
+        <v>2205</v>
+      </c>
+      <c r="L4">
+        <v>2223</v>
+      </c>
+      <c r="M4">
+        <v>2182</v>
+      </c>
+      <c r="N4">
+        <v>1978</v>
+      </c>
+      <c r="O4">
+        <v>1999</v>
+      </c>
+      <c r="P4">
+        <v>1574</v>
+      </c>
+      <c r="Q4">
+        <v>1265</v>
+      </c>
+      <c r="R4">
+        <v>902</v>
+      </c>
+      <c r="S4">
+        <v>838</v>
+      </c>
+      <c r="T4">
+        <v>680</v>
+      </c>
+      <c r="U4">
+        <v>911</v>
+      </c>
+      <c r="V4">
+        <v>31926</v>
+      </c>
+      <c r="X4" s="19">
+        <v>2015</v>
+      </c>
+      <c r="Y4">
+        <f t="shared" ref="Y4:Y7" si="0">SUM(D4:G4)</f>
+        <v>7545</v>
+      </c>
+      <c r="Z4">
+        <f t="shared" ref="Z4:Z7" si="1">SUM(H4:Q4)</f>
+        <v>21050</v>
+      </c>
+      <c r="AA4">
+        <f t="shared" ref="AA4:AA7" si="2">SUM(R4:U4)</f>
+        <v>3331</v>
+      </c>
+      <c r="AC4" s="19">
+        <v>2015</v>
+      </c>
+      <c r="AD4" s="7">
+        <f>(Y4/Y3)-1</f>
+        <v>0.1400725294650953</v>
+      </c>
+      <c r="AE4" s="7">
+        <f t="shared" ref="AE4:AF4" si="3">(Z4/Z3)-1</f>
+        <v>0.118490967056323</v>
+      </c>
+      <c r="AF4" s="7">
+        <f t="shared" si="3"/>
+        <v>7.2440437862202112E-2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B5">
+        <v>2020</v>
+      </c>
+      <c r="C5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D5">
+        <v>2286</v>
+      </c>
+      <c r="E5">
+        <v>2276</v>
+      </c>
+      <c r="F5">
+        <v>1965</v>
+      </c>
+      <c r="G5">
+        <v>1889</v>
+      </c>
+      <c r="H5">
+        <v>2214</v>
+      </c>
+      <c r="I5">
+        <v>2706</v>
+      </c>
+      <c r="J5">
+        <v>3058</v>
+      </c>
+      <c r="K5">
+        <v>2747</v>
+      </c>
+      <c r="L5">
+        <v>2274</v>
+      </c>
+      <c r="M5">
+        <v>2168</v>
+      </c>
+      <c r="N5">
+        <v>2104</v>
+      </c>
+      <c r="O5">
+        <v>1903</v>
+      </c>
+      <c r="P5">
+        <v>1917</v>
+      </c>
+      <c r="Q5">
+        <v>1514</v>
+      </c>
+      <c r="R5">
+        <v>1205</v>
+      </c>
+      <c r="S5">
+        <v>830</v>
+      </c>
+      <c r="T5">
+        <v>706</v>
+      </c>
+      <c r="U5">
+        <v>936</v>
+      </c>
+      <c r="V5">
+        <v>34698</v>
+      </c>
+      <c r="X5" s="19">
+        <v>2020</v>
+      </c>
+      <c r="Y5">
+        <f t="shared" si="0"/>
+        <v>8416</v>
+      </c>
+      <c r="Z5">
+        <f t="shared" si="1"/>
+        <v>22605</v>
+      </c>
+      <c r="AA5">
+        <f t="shared" si="2"/>
+        <v>3677</v>
+      </c>
+      <c r="AC5" s="19">
+        <v>2020</v>
+      </c>
+      <c r="AD5" s="7">
+        <f t="shared" ref="AD5:AD7" si="4">(Y5/Y4)-1</f>
+        <v>0.11544068919814454</v>
+      </c>
+      <c r="AE5" s="7">
+        <f t="shared" ref="AE5:AE7" si="5">(Z5/Z4)-1</f>
+        <v>7.3871733966745845E-2</v>
+      </c>
+      <c r="AF5" s="7">
+        <f t="shared" ref="AF5:AF7" si="6">(AA5/AA4)-1</f>
+        <v>0.10387271089762828</v>
+      </c>
+    </row>
+    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>58</v>
+      </c>
+      <c r="B6">
+        <v>2025</v>
+      </c>
+      <c r="C6" t="s">
+        <v>22</v>
+      </c>
+      <c r="D6">
+        <v>2357</v>
+      </c>
+      <c r="E6">
+        <v>2384</v>
+      </c>
+      <c r="F6">
+        <v>2339</v>
+      </c>
+      <c r="G6">
+        <v>2200</v>
+      </c>
+      <c r="H6">
+        <v>2213</v>
+      </c>
+      <c r="I6">
+        <v>2727</v>
+      </c>
+      <c r="J6">
+        <v>2999</v>
+      </c>
+      <c r="K6">
+        <v>3117</v>
+      </c>
+      <c r="L6">
+        <v>2793</v>
+      </c>
+      <c r="M6">
+        <v>2194</v>
+      </c>
+      <c r="N6">
+        <v>2071</v>
+      </c>
+      <c r="O6">
+        <v>2004</v>
+      </c>
+      <c r="P6">
+        <v>1804</v>
+      </c>
+      <c r="Q6">
+        <v>1823</v>
+      </c>
+      <c r="R6">
+        <v>1420</v>
+      </c>
+      <c r="S6">
+        <v>1089</v>
+      </c>
+      <c r="T6">
+        <v>689</v>
+      </c>
+      <c r="U6">
+        <v>971</v>
+      </c>
+      <c r="V6">
+        <v>37194</v>
+      </c>
+      <c r="X6" s="19">
+        <v>2025</v>
+      </c>
+      <c r="Y6">
+        <f t="shared" si="0"/>
+        <v>9280</v>
+      </c>
+      <c r="Z6">
+        <f t="shared" si="1"/>
+        <v>23745</v>
+      </c>
+      <c r="AA6">
+        <f t="shared" si="2"/>
+        <v>4169</v>
+      </c>
+      <c r="AC6" s="19">
+        <v>2025</v>
+      </c>
+      <c r="AD6" s="7">
+        <f t="shared" si="4"/>
+        <v>0.10266159695817501</v>
+      </c>
+      <c r="AE6" s="7">
+        <f t="shared" si="5"/>
+        <v>5.0431320504313204E-2</v>
+      </c>
+      <c r="AF6" s="7">
+        <f t="shared" si="6"/>
+        <v>0.13380473211857491</v>
+      </c>
+    </row>
+    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>58</v>
+      </c>
+      <c r="B7">
+        <v>2030</v>
+      </c>
+      <c r="C7" t="s">
+        <v>22</v>
+      </c>
+      <c r="D7">
+        <v>2391</v>
+      </c>
+      <c r="E7">
+        <v>2409</v>
+      </c>
+      <c r="F7">
+        <v>2399</v>
+      </c>
+      <c r="G7">
+        <v>2550</v>
+      </c>
+      <c r="H7">
+        <v>2486</v>
+      </c>
+      <c r="I7">
+        <v>2685</v>
+      </c>
+      <c r="J7">
+        <v>2981</v>
+      </c>
+      <c r="K7">
+        <v>3015</v>
+      </c>
+      <c r="L7">
+        <v>3115</v>
+      </c>
+      <c r="M7">
+        <v>2643</v>
+      </c>
+      <c r="N7">
+        <v>2048</v>
+      </c>
+      <c r="O7">
+        <v>1926</v>
+      </c>
+      <c r="P7">
+        <v>1857</v>
+      </c>
+      <c r="Q7">
+        <v>1672</v>
+      </c>
+      <c r="R7">
+        <v>1674</v>
+      </c>
+      <c r="S7">
+        <v>1248</v>
+      </c>
+      <c r="T7">
+        <v>872</v>
+      </c>
+      <c r="U7">
+        <v>969</v>
+      </c>
+      <c r="V7">
+        <v>38940</v>
+      </c>
+      <c r="X7" s="19">
+        <v>2030</v>
+      </c>
+      <c r="Y7">
+        <f t="shared" si="0"/>
+        <v>9749</v>
+      </c>
+      <c r="Z7">
+        <f t="shared" si="1"/>
+        <v>24428</v>
+      </c>
+      <c r="AA7">
+        <f t="shared" si="2"/>
+        <v>4763</v>
+      </c>
+      <c r="AC7" s="19">
+        <v>2030</v>
+      </c>
+      <c r="AD7" s="7">
+        <f t="shared" si="4"/>
+        <v>5.0538793103448221E-2</v>
+      </c>
+      <c r="AE7" s="7">
+        <f t="shared" si="5"/>
+        <v>2.8763950305327413E-2</v>
+      </c>
+      <c r="AF7" s="7">
+        <f t="shared" si="6"/>
+        <v>0.14248021108179421</v>
+      </c>
+    </row>
+    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD8" s="7"/>
+      <c r="AE8" s="7"/>
+      <c r="AF8" s="7"/>
+    </row>
+    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA9" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB9" s="18"/>
+      <c r="AD9" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE9" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF9" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>56</v>
+      </c>
+      <c r="B10">
+        <v>2010</v>
+      </c>
+      <c r="C10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D10">
+        <v>1978</v>
+      </c>
+      <c r="E10">
+        <v>1806</v>
+      </c>
+      <c r="F10">
+        <v>1710</v>
+      </c>
+      <c r="G10">
+        <v>1893</v>
+      </c>
+      <c r="H10">
+        <v>2027</v>
+      </c>
+      <c r="I10">
+        <v>1962</v>
+      </c>
+      <c r="J10">
+        <v>1567</v>
+      </c>
+      <c r="K10">
+        <v>1507</v>
+      </c>
+      <c r="L10">
+        <v>1584</v>
+      </c>
+      <c r="M10">
+        <v>1630</v>
+      </c>
+      <c r="N10">
+        <v>1499</v>
+      </c>
+      <c r="O10">
+        <v>1272</v>
+      </c>
+      <c r="P10">
+        <v>1132</v>
+      </c>
+      <c r="Q10">
+        <v>1002</v>
+      </c>
+      <c r="R10">
+        <v>971</v>
+      </c>
+      <c r="S10">
+        <v>966</v>
+      </c>
+      <c r="T10">
+        <v>764</v>
+      </c>
+      <c r="U10">
+        <v>479</v>
+      </c>
+      <c r="V10">
+        <v>25749</v>
+      </c>
+      <c r="X10" s="19">
+        <v>2010</v>
+      </c>
+      <c r="Y10">
+        <f>SUM(D10:G10)</f>
+        <v>7387</v>
+      </c>
+      <c r="Z10">
+        <f>SUM(H10:Q10)</f>
+        <v>15182</v>
+      </c>
+      <c r="AA10">
+        <f>SUM(R10:U10)</f>
+        <v>3180</v>
+      </c>
+      <c r="AC10" s="19">
+        <v>2010</v>
+      </c>
+      <c r="AD10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE10" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF10" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>56</v>
+      </c>
+      <c r="B11">
+        <v>2015</v>
+      </c>
+      <c r="C11" t="s">
+        <v>22</v>
+      </c>
+      <c r="D11">
+        <v>2072</v>
+      </c>
+      <c r="E11">
+        <v>1894</v>
+      </c>
+      <c r="F11">
+        <v>1719</v>
+      </c>
+      <c r="G11">
+        <v>1712</v>
+      </c>
+      <c r="H11">
+        <v>1813</v>
+      </c>
+      <c r="I11">
+        <v>2057</v>
+      </c>
+      <c r="J11">
+        <v>1889</v>
+      </c>
+      <c r="K11">
+        <v>1562</v>
+      </c>
+      <c r="L11">
+        <v>1486</v>
+      </c>
+      <c r="M11">
+        <v>1549</v>
+      </c>
+      <c r="N11">
+        <v>1578</v>
+      </c>
+      <c r="O11">
+        <v>1453</v>
+      </c>
+      <c r="P11">
+        <v>1232</v>
+      </c>
+      <c r="Q11">
+        <v>1101</v>
+      </c>
+      <c r="R11">
+        <v>968</v>
+      </c>
+      <c r="S11">
+        <v>895</v>
+      </c>
+      <c r="T11">
+        <v>774</v>
+      </c>
+      <c r="U11">
+        <v>700</v>
+      </c>
+      <c r="V11">
+        <v>26454</v>
+      </c>
+      <c r="X11" s="19">
+        <v>2015</v>
+      </c>
+      <c r="Y11">
+        <f t="shared" ref="Y11:Y14" si="7">SUM(D11:G11)</f>
+        <v>7397</v>
+      </c>
+      <c r="Z11">
+        <f t="shared" ref="Z11:Z14" si="8">SUM(H11:Q11)</f>
+        <v>15720</v>
+      </c>
+      <c r="AA11">
+        <f t="shared" ref="AA11:AA14" si="9">SUM(R11:U11)</f>
+        <v>3337</v>
+      </c>
+      <c r="AC11" s="19">
+        <v>2015</v>
+      </c>
+      <c r="AD11" s="7">
+        <f>(Y11/Y10)-1</f>
+        <v>1.3537295248409187E-3</v>
+      </c>
+      <c r="AE11" s="7">
+        <f t="shared" ref="AE11:AE14" si="10">(Z11/Z10)-1</f>
+        <v>3.5436701356869937E-2</v>
+      </c>
+      <c r="AF11" s="7">
+        <f t="shared" ref="AF11:AF14" si="11">(AA11/AA10)-1</f>
+        <v>4.9371069182389871E-2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>56</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12" t="s">
+        <v>22</v>
+      </c>
+      <c r="D12">
+        <v>1933</v>
+      </c>
+      <c r="E12">
+        <v>1979</v>
+      </c>
+      <c r="F12">
+        <v>1799</v>
+      </c>
+      <c r="G12">
+        <v>1713</v>
+      </c>
+      <c r="H12">
+        <v>1645</v>
+      </c>
+      <c r="I12">
+        <v>1879</v>
+      </c>
+      <c r="J12">
+        <v>1992</v>
+      </c>
+      <c r="K12">
+        <v>1863</v>
+      </c>
+      <c r="L12">
+        <v>1547</v>
+      </c>
+      <c r="M12">
+        <v>1462</v>
+      </c>
+      <c r="N12">
+        <v>1505</v>
+      </c>
+      <c r="O12">
+        <v>1532</v>
+      </c>
+      <c r="P12">
+        <v>1407</v>
+      </c>
+      <c r="Q12">
+        <v>1199</v>
+      </c>
+      <c r="R12">
+        <v>1065</v>
+      </c>
+      <c r="S12">
+        <v>907</v>
+      </c>
+      <c r="T12">
+        <v>734</v>
+      </c>
+      <c r="U12">
+        <v>820</v>
+      </c>
+      <c r="V12">
+        <v>26981</v>
+      </c>
+      <c r="X12" s="19">
+        <v>2020</v>
+      </c>
+      <c r="Y12">
+        <f t="shared" si="7"/>
+        <v>7424</v>
+      </c>
+      <c r="Z12">
+        <f t="shared" si="8"/>
+        <v>16031</v>
+      </c>
+      <c r="AA12">
+        <f t="shared" si="9"/>
+        <v>3526</v>
+      </c>
+      <c r="AC12" s="19">
+        <v>2020</v>
+      </c>
+      <c r="AD12" s="7">
+        <f t="shared" ref="AD12:AD14" si="12">(Y12/Y11)-1</f>
+        <v>3.6501284304448767E-3</v>
+      </c>
+      <c r="AE12" s="7">
+        <f t="shared" si="10"/>
+        <v>1.9783715012722691E-2</v>
+      </c>
+      <c r="AF12" s="7">
+        <f t="shared" si="11"/>
+        <v>5.6637698531615266E-2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>56</v>
+      </c>
+      <c r="B13">
+        <v>2025</v>
+      </c>
+      <c r="C13" t="s">
+        <v>22</v>
+      </c>
+      <c r="D13">
+        <v>1826</v>
+      </c>
+      <c r="E13">
+        <v>1861</v>
+      </c>
+      <c r="F13">
+        <v>1878</v>
+      </c>
+      <c r="G13">
+        <v>1778</v>
+      </c>
+      <c r="H13">
+        <v>1625</v>
+      </c>
+      <c r="I13">
+        <v>1723</v>
+      </c>
+      <c r="J13">
+        <v>1843</v>
+      </c>
+      <c r="K13">
+        <v>1967</v>
+      </c>
+      <c r="L13">
+        <v>1836</v>
+      </c>
+      <c r="M13">
+        <v>1527</v>
+      </c>
+      <c r="N13">
+        <v>1430</v>
+      </c>
+      <c r="O13">
+        <v>1467</v>
+      </c>
+      <c r="P13">
+        <v>1492</v>
+      </c>
+      <c r="Q13">
+        <v>1376</v>
+      </c>
+      <c r="R13">
+        <v>1164</v>
+      </c>
+      <c r="S13">
+        <v>1006</v>
+      </c>
+      <c r="T13">
+        <v>765</v>
+      </c>
+      <c r="U13">
+        <v>878</v>
+      </c>
+      <c r="V13">
+        <v>27442</v>
+      </c>
+      <c r="X13" s="19">
+        <v>2025</v>
+      </c>
+      <c r="Y13">
+        <f t="shared" si="7"/>
+        <v>7343</v>
+      </c>
+      <c r="Z13">
+        <f t="shared" si="8"/>
+        <v>16286</v>
+      </c>
+      <c r="AA13">
+        <f t="shared" si="9"/>
+        <v>3813</v>
+      </c>
+      <c r="AC13" s="19">
+        <v>2025</v>
+      </c>
+      <c r="AD13" s="7">
+        <f t="shared" si="12"/>
+        <v>-1.0910560344827624E-2</v>
+      </c>
+      <c r="AE13" s="7">
+        <f t="shared" si="10"/>
+        <v>1.5906680805938489E-2</v>
+      </c>
+      <c r="AF13" s="7">
+        <f t="shared" si="11"/>
+        <v>8.1395348837209225E-2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>56</v>
+      </c>
+      <c r="B14">
+        <v>2030</v>
+      </c>
+      <c r="C14" t="s">
+        <v>22</v>
+      </c>
+      <c r="D14">
+        <v>1755</v>
+      </c>
+      <c r="E14">
+        <v>1753</v>
+      </c>
+      <c r="F14">
+        <v>1759</v>
+      </c>
+      <c r="G14">
+        <v>1832</v>
+      </c>
+      <c r="H14">
+        <v>1648</v>
+      </c>
+      <c r="I14">
+        <v>1701</v>
+      </c>
+      <c r="J14">
+        <v>1687</v>
+      </c>
+      <c r="K14">
+        <v>1818</v>
+      </c>
+      <c r="L14">
+        <v>1927</v>
+      </c>
+      <c r="M14">
+        <v>1795</v>
+      </c>
+      <c r="N14">
+        <v>1487</v>
+      </c>
+      <c r="O14">
+        <v>1392</v>
+      </c>
+      <c r="P14">
+        <v>1424</v>
+      </c>
+      <c r="Q14">
+        <v>1459</v>
+      </c>
+      <c r="R14">
+        <v>1335</v>
+      </c>
+      <c r="S14">
+        <v>1099</v>
+      </c>
+      <c r="T14">
+        <v>848</v>
+      </c>
+      <c r="U14">
+        <v>955</v>
+      </c>
+      <c r="V14">
+        <v>27674</v>
+      </c>
+      <c r="X14" s="19">
+        <v>2030</v>
+      </c>
+      <c r="Y14">
+        <f t="shared" si="7"/>
+        <v>7099</v>
+      </c>
+      <c r="Z14">
+        <f t="shared" si="8"/>
+        <v>16338</v>
+      </c>
+      <c r="AA14">
+        <f t="shared" si="9"/>
+        <v>4237</v>
+      </c>
+      <c r="AC14" s="19">
+        <v>2030</v>
+      </c>
+      <c r="AD14" s="7">
+        <f t="shared" si="12"/>
+        <v>-3.3228925507285845E-2</v>
+      </c>
+      <c r="AE14" s="7">
+        <f t="shared" si="10"/>
+        <v>3.1929264398871116E-3</v>
+      </c>
+      <c r="AF14" s="7">
+        <f t="shared" si="11"/>
+        <v>0.11119853134015201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="AD15" s="7"/>
+      <c r="AE15" s="7"/>
+      <c r="AF15" s="7"/>
+    </row>
+    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="Y16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="Z16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AA16" s="18" t="s">
+        <v>43</v>
+      </c>
+      <c r="AB16" s="18"/>
+      <c r="AD16" s="18" t="s">
+        <v>41</v>
+      </c>
+      <c r="AE16" s="18" t="s">
+        <v>42</v>
+      </c>
+      <c r="AF16" s="18" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>57</v>
+      </c>
+      <c r="B17">
+        <v>2010</v>
+      </c>
+      <c r="C17" t="s">
+        <v>22</v>
+      </c>
+      <c r="D17">
+        <v>301</v>
+      </c>
+      <c r="E17">
+        <v>379</v>
+      </c>
+      <c r="F17">
+        <v>394</v>
+      </c>
+      <c r="G17">
+        <v>481</v>
+      </c>
+      <c r="H17">
+        <v>547</v>
+      </c>
+      <c r="I17">
+        <v>395</v>
+      </c>
+      <c r="J17">
+        <v>320</v>
+      </c>
+      <c r="K17">
+        <v>404</v>
+      </c>
+      <c r="L17">
+        <v>511</v>
+      </c>
+      <c r="M17">
+        <v>459</v>
+      </c>
+      <c r="N17">
+        <v>514</v>
+      </c>
+      <c r="O17">
+        <v>518</v>
+      </c>
+      <c r="P17">
+        <v>527</v>
+      </c>
+      <c r="Q17">
+        <v>374</v>
+      </c>
+      <c r="R17">
+        <v>374</v>
+      </c>
+      <c r="S17">
+        <v>264</v>
+      </c>
+      <c r="T17">
+        <v>278</v>
+      </c>
+      <c r="U17">
+        <v>268</v>
+      </c>
+      <c r="V17">
+        <v>7308</v>
+      </c>
+      <c r="X17" s="19">
+        <v>2010</v>
+      </c>
+      <c r="Y17">
+        <f>SUM(D17:G17)</f>
+        <v>1555</v>
+      </c>
+      <c r="Z17">
+        <f>SUM(H17:Q17)</f>
+        <v>4569</v>
+      </c>
+      <c r="AA17">
+        <f>SUM(R17:U17)</f>
+        <v>1184</v>
+      </c>
+      <c r="AC17" s="19">
+        <v>2010</v>
+      </c>
+      <c r="AD17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AE17" s="7">
+        <v>0</v>
+      </c>
+      <c r="AF17" s="7">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>57</v>
+      </c>
+      <c r="B18">
+        <v>2015</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>306</v>
+      </c>
+      <c r="E18">
+        <v>391</v>
+      </c>
+      <c r="F18">
+        <v>414</v>
+      </c>
+      <c r="G18">
+        <v>447</v>
+      </c>
+      <c r="H18">
+        <v>559</v>
+      </c>
+      <c r="I18">
+        <v>367</v>
+      </c>
+      <c r="J18">
+        <v>356</v>
+      </c>
+      <c r="K18">
+        <v>363</v>
+      </c>
+      <c r="L18">
+        <v>454</v>
+      </c>
+      <c r="M18">
+        <v>495</v>
+      </c>
+      <c r="N18">
+        <v>473</v>
+      </c>
+      <c r="O18">
+        <v>494</v>
+      </c>
+      <c r="P18">
+        <v>496</v>
+      </c>
+      <c r="Q18">
+        <v>481</v>
+      </c>
+      <c r="R18">
+        <v>392</v>
+      </c>
+      <c r="S18">
+        <v>322</v>
+      </c>
+      <c r="T18">
+        <v>219</v>
+      </c>
+      <c r="U18">
+        <v>324</v>
+      </c>
+      <c r="V18">
+        <v>7353</v>
+      </c>
+      <c r="X18" s="19">
+        <v>2015</v>
+      </c>
+      <c r="Y18">
+        <f t="shared" ref="Y18:Y21" si="13">SUM(D18:G18)</f>
+        <v>1558</v>
+      </c>
+      <c r="Z18">
+        <f t="shared" ref="Z18:Z21" si="14">SUM(H18:Q18)</f>
+        <v>4538</v>
+      </c>
+      <c r="AA18">
+        <f t="shared" ref="AA18:AA21" si="15">SUM(R18:U18)</f>
+        <v>1257</v>
+      </c>
+      <c r="AC18" s="19">
+        <v>2015</v>
+      </c>
+      <c r="AD18" s="7">
+        <f>(Y18/Y17)-1</f>
+        <v>1.9292604501608412E-3</v>
+      </c>
+      <c r="AE18" s="7">
+        <f t="shared" ref="AE18:AE21" si="16">(Z18/Z17)-1</f>
+        <v>-6.7848544539286237E-3</v>
+      </c>
+      <c r="AF18" s="7">
+        <f t="shared" ref="AF18:AF21" si="17">(AA18/AA17)-1</f>
+        <v>6.1655405405405483E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>57</v>
+      </c>
+      <c r="B19">
+        <v>2020</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>298</v>
+      </c>
+      <c r="E19">
+        <v>367</v>
+      </c>
+      <c r="F19">
+        <v>429</v>
+      </c>
+      <c r="G19">
+        <v>476</v>
+      </c>
+      <c r="H19">
+        <v>494</v>
+      </c>
+      <c r="I19">
+        <v>432</v>
+      </c>
+      <c r="J19">
+        <v>319</v>
+      </c>
+      <c r="K19">
+        <v>384</v>
+      </c>
+      <c r="L19">
+        <v>410</v>
+      </c>
+      <c r="M19">
+        <v>444</v>
+      </c>
+      <c r="N19">
+        <v>502</v>
+      </c>
+      <c r="O19">
+        <v>456</v>
+      </c>
+      <c r="P19">
+        <v>474</v>
+      </c>
+      <c r="Q19">
+        <v>455</v>
+      </c>
+      <c r="R19">
+        <v>505</v>
+      </c>
+      <c r="S19">
+        <v>344</v>
+      </c>
+      <c r="T19">
+        <v>273</v>
+      </c>
+      <c r="U19">
+        <v>321</v>
+      </c>
+      <c r="V19">
+        <v>7383</v>
+      </c>
+      <c r="X19" s="19">
+        <v>2020</v>
+      </c>
+      <c r="Y19">
+        <f t="shared" si="13"/>
+        <v>1570</v>
+      </c>
+      <c r="Z19">
+        <f t="shared" si="14"/>
+        <v>4370</v>
+      </c>
+      <c r="AA19">
+        <f t="shared" si="15"/>
+        <v>1443</v>
+      </c>
+      <c r="AC19" s="19">
+        <v>2020</v>
+      </c>
+      <c r="AD19" s="7">
+        <f t="shared" ref="AD19:AD21" si="18">(Y19/Y18)-1</f>
+        <v>7.7021822849807631E-3</v>
+      </c>
+      <c r="AE19" s="7">
+        <f t="shared" si="16"/>
+        <v>-3.7020713970912333E-2</v>
+      </c>
+      <c r="AF19" s="7">
+        <f t="shared" si="17"/>
+        <v>0.14797136038186154</v>
+      </c>
+    </row>
+    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>57</v>
+      </c>
+      <c r="B20">
+        <v>2025</v>
+      </c>
+      <c r="C20" t="s">
+        <v>22</v>
+      </c>
+      <c r="D20">
+        <v>297</v>
+      </c>
+      <c r="E20">
+        <v>360</v>
+      </c>
+      <c r="F20">
+        <v>400</v>
+      </c>
+      <c r="G20">
+        <v>486</v>
+      </c>
+      <c r="H20">
+        <v>518</v>
+      </c>
+      <c r="I20">
+        <v>385</v>
+      </c>
+      <c r="J20">
+        <v>379</v>
+      </c>
+      <c r="K20">
+        <v>344</v>
+      </c>
+      <c r="L20">
+        <v>433</v>
+      </c>
+      <c r="M20">
+        <v>402</v>
+      </c>
+      <c r="N20">
+        <v>452</v>
+      </c>
+      <c r="O20">
+        <v>485</v>
+      </c>
+      <c r="P20">
+        <v>441</v>
+      </c>
+      <c r="Q20">
+        <v>437</v>
+      </c>
+      <c r="R20">
+        <v>480</v>
+      </c>
+      <c r="S20">
+        <v>447</v>
+      </c>
+      <c r="T20">
+        <v>301</v>
+      </c>
+      <c r="U20">
+        <v>367</v>
+      </c>
+      <c r="V20">
+        <v>7414</v>
+      </c>
+      <c r="X20" s="19">
+        <v>2025</v>
+      </c>
+      <c r="Y20">
+        <f t="shared" si="13"/>
+        <v>1543</v>
+      </c>
+      <c r="Z20">
+        <f t="shared" si="14"/>
+        <v>4276</v>
+      </c>
+      <c r="AA20">
+        <f t="shared" si="15"/>
+        <v>1595</v>
+      </c>
+      <c r="AC20" s="19">
+        <v>2025</v>
+      </c>
+      <c r="AD20" s="7">
+        <f t="shared" si="18"/>
+        <v>-1.7197452229299359E-2</v>
+      </c>
+      <c r="AE20" s="7">
+        <f t="shared" si="16"/>
+        <v>-2.1510297482837504E-2</v>
+      </c>
+      <c r="AF20" s="7">
+        <f t="shared" si="17"/>
+        <v>0.10533610533610527</v>
+      </c>
+    </row>
+    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>57</v>
+      </c>
+      <c r="B21">
+        <v>2030</v>
+      </c>
+      <c r="C21" t="s">
+        <v>22</v>
+      </c>
+      <c r="D21">
+        <v>302</v>
+      </c>
+      <c r="E21">
+        <v>357</v>
+      </c>
+      <c r="F21">
+        <v>392</v>
+      </c>
+      <c r="G21">
+        <v>451</v>
+      </c>
+      <c r="H21">
+        <v>520</v>
+      </c>
+      <c r="I21">
+        <v>405</v>
+      </c>
+      <c r="J21">
+        <v>338</v>
+      </c>
+      <c r="K21">
+        <v>410</v>
+      </c>
+      <c r="L21">
+        <v>386</v>
+      </c>
+      <c r="M21">
+        <v>422</v>
+      </c>
+      <c r="N21">
+        <v>409</v>
+      </c>
+      <c r="O21">
+        <v>438</v>
+      </c>
+      <c r="P21">
+        <v>471</v>
+      </c>
+      <c r="Q21">
+        <v>408</v>
+      </c>
+      <c r="R21">
+        <v>464</v>
+      </c>
+      <c r="S21">
+        <v>429</v>
+      </c>
+      <c r="T21">
+        <v>394</v>
+      </c>
+      <c r="U21">
+        <v>428</v>
+      </c>
+      <c r="V21">
+        <v>7424</v>
+      </c>
+      <c r="X21" s="19">
+        <v>2030</v>
+      </c>
+      <c r="Y21">
+        <f t="shared" si="13"/>
+        <v>1502</v>
+      </c>
+      <c r="Z21">
+        <f t="shared" si="14"/>
+        <v>4207</v>
+      </c>
+      <c r="AA21">
+        <f t="shared" si="15"/>
+        <v>1715</v>
+      </c>
+      <c r="AC21" s="19">
+        <v>2030</v>
+      </c>
+      <c r="AD21" s="7">
+        <f t="shared" si="18"/>
+        <v>-2.6571613739468591E-2</v>
+      </c>
+      <c r="AE21" s="7">
+        <f t="shared" si="16"/>
+        <v>-1.6136576239476175E-2</v>
+      </c>
+      <c r="AF21" s="7">
+        <f t="shared" si="17"/>
+        <v>7.5235109717868287E-2</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P82"/>
   <sheetViews>
@@ -2170,22 +3859,22 @@
       <c r="I24">
         <v>1485588</v>
       </c>
-      <c r="L24" s="11">
+      <c r="L24" s="7">
         <v>0</v>
       </c>
-      <c r="M24" s="11">
+      <c r="M24" s="7">
         <f>(F24/E24)-1</f>
         <v>4.1735894859371347E-2</v>
       </c>
-      <c r="N24" s="11">
+      <c r="N24" s="7">
         <f t="shared" ref="N24" si="0">(G24/F24)-1</f>
         <v>5.9450248946276041E-2</v>
       </c>
-      <c r="O24" s="11">
+      <c r="O24" s="7">
         <f t="shared" ref="O24" si="1">(H24/G24)-1</f>
         <v>5.9369964580696211E-2</v>
       </c>
-      <c r="P24" s="11">
+      <c r="P24" s="7">
         <f t="shared" ref="P24" si="2">(I24/H24)-1</f>
         <v>5.3438167445264195E-2</v>
       </c>
@@ -2223,22 +3912,22 @@
       <c r="K26" t="s">
         <v>41</v>
       </c>
-      <c r="L26" s="11">
+      <c r="L26" s="7">
         <v>0</v>
       </c>
-      <c r="M26" s="11">
+      <c r="M26" s="7">
         <f>(F26/E26)-1</f>
         <v>3.9401588807624011E-2</v>
       </c>
-      <c r="N26" s="11">
+      <c r="N26" s="7">
         <f t="shared" ref="N26:P26" si="4">(G26/F26)-1</f>
         <v>6.9402479814872908E-2</v>
       </c>
-      <c r="O26" s="11">
+      <c r="O26" s="7">
         <f t="shared" si="4"/>
         <v>7.6814045564931543E-2</v>
       </c>
-      <c r="P26" s="11">
+      <c r="P26" s="7">
         <f t="shared" si="4"/>
         <v>5.5881217311944953E-2</v>
       </c>
@@ -2270,22 +3959,22 @@
       <c r="K27" t="s">
         <v>42</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="7">
         <v>0</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="7">
         <f t="shared" ref="M27:M28" si="6">(F27/E27)-1</f>
         <v>3.5243830962851552E-2</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="7">
         <f t="shared" ref="N27:N28" si="7">(G27/F27)-1</f>
         <v>3.5602441450624411E-2</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="7">
         <f t="shared" ref="O27:O28" si="8">(H27/G27)-1</f>
         <v>3.4733059791760557E-2</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P27" s="7">
         <f t="shared" ref="P27:P28" si="9">(I27/H27)-1</f>
         <v>3.4814090669979647E-2</v>
       </c>
@@ -2317,22 +4006,22 @@
       <c r="K28" t="s">
         <v>43</v>
       </c>
-      <c r="L28" s="11">
+      <c r="L28" s="7">
         <v>0</v>
       </c>
-      <c r="M28" s="11">
+      <c r="M28" s="7">
         <f t="shared" si="6"/>
         <v>8.4823561022211669E-2</v>
       </c>
-      <c r="N28" s="11">
+      <c r="N28" s="7">
         <f t="shared" si="7"/>
         <v>0.17272220655112869</v>
       </c>
-      <c r="O28" s="11">
+      <c r="O28" s="7">
         <f t="shared" si="8"/>
         <v>0.14876154270360331</v>
       </c>
-      <c r="P28" s="11">
+      <c r="P28" s="7">
         <f t="shared" si="9"/>
         <v>0.13216315733028283</v>
       </c>
@@ -2883,22 +4572,22 @@
       <c r="I51">
         <v>734090</v>
       </c>
-      <c r="L51" s="11">
+      <c r="L51" s="7">
         <v>0</v>
       </c>
-      <c r="M51" s="11">
+      <c r="M51" s="7">
         <f>(F51/E51)-1</f>
         <v>4.3574958952837584E-2</v>
       </c>
-      <c r="N51" s="11">
+      <c r="N51" s="7">
         <f t="shared" ref="N51" si="11">(G51/F51)-1</f>
         <v>6.129514224638366E-2</v>
       </c>
-      <c r="O51" s="11">
+      <c r="O51" s="7">
         <f t="shared" ref="O51" si="12">(H51/G51)-1</f>
         <v>6.0750433082803035E-2</v>
       </c>
-      <c r="P51" s="11">
+      <c r="P51" s="7">
         <f t="shared" ref="P51" si="13">(I51/H51)-1</f>
         <v>5.440281292820881E-2</v>
       </c>
@@ -2936,22 +4625,22 @@
       <c r="K53" t="s">
         <v>41</v>
       </c>
-      <c r="L53" s="11">
+      <c r="L53" s="7">
         <v>0</v>
       </c>
-      <c r="M53" s="11">
+      <c r="M53" s="7">
         <f>(F53/E53)-1</f>
         <v>3.9688261750266074E-2</v>
       </c>
-      <c r="N53" s="11">
+      <c r="N53" s="7">
         <f t="shared" ref="N53:N55" si="15">(G53/F53)-1</f>
         <v>7.0158174553379693E-2</v>
       </c>
-      <c r="O53" s="11">
+      <c r="O53" s="7">
         <f t="shared" ref="O53:O55" si="16">(H53/G53)-1</f>
         <v>7.7450968291388422E-2</v>
       </c>
-      <c r="P53" s="11">
+      <c r="P53" s="7">
         <f t="shared" ref="P53:P55" si="17">(I53/H53)-1</f>
         <v>5.7781749032006724E-2</v>
       </c>
@@ -2983,22 +4672,22 @@
       <c r="K54" t="s">
         <v>42</v>
       </c>
-      <c r="L54" s="11">
+      <c r="L54" s="7">
         <v>0</v>
       </c>
-      <c r="M54" s="11">
+      <c r="M54" s="7">
         <f t="shared" ref="M54:M55" si="19">(F54/E54)-1</f>
         <v>3.5372988598534549E-2</v>
       </c>
-      <c r="N54" s="11">
+      <c r="N54" s="7">
         <f t="shared" si="15"/>
         <v>3.6647063482634357E-2</v>
       </c>
-      <c r="O54" s="11">
+      <c r="O54" s="7">
         <f t="shared" si="16"/>
         <v>3.7077803935800846E-2</v>
       </c>
-      <c r="P54" s="11">
+      <c r="P54" s="7">
         <f t="shared" si="17"/>
         <v>3.6854985944547058E-2</v>
       </c>
@@ -3030,22 +4719,22 @@
       <c r="K55" t="s">
         <v>43</v>
       </c>
-      <c r="L55" s="11">
+      <c r="L55" s="7">
         <v>0</v>
       </c>
-      <c r="M55" s="11">
+      <c r="M55" s="7">
         <f t="shared" si="19"/>
         <v>0.10993076475873376</v>
       </c>
-      <c r="N55" s="11">
+      <c r="N55" s="7">
         <f t="shared" si="15"/>
         <v>0.19805406091773414</v>
       </c>
-      <c r="O55" s="11">
+      <c r="O55" s="7">
         <f t="shared" si="16"/>
         <v>0.15625124203441931</v>
       </c>
-      <c r="P55" s="11">
+      <c r="P55" s="7">
         <f t="shared" si="17"/>
         <v>0.13497565167573766</v>
       </c>
@@ -3596,22 +5285,22 @@
       <c r="I78">
         <v>751498</v>
       </c>
-      <c r="L78" s="11">
+      <c r="L78" s="7">
         <v>0</v>
       </c>
-      <c r="M78" s="11">
+      <c r="M78" s="7">
         <f>(F78/E78)-1</f>
         <v>3.9959579166972237E-2</v>
       </c>
-      <c r="N78" s="11">
+      <c r="N78" s="7">
         <f t="shared" ref="N78" si="21">(G78/F78)-1</f>
         <v>5.7662108071002471E-2</v>
       </c>
-      <c r="O78" s="11">
+      <c r="O78" s="7">
         <f t="shared" ref="O78" si="22">(H78/G78)-1</f>
         <v>5.8027365919147034E-2</v>
       </c>
-      <c r="P78" s="11">
+      <c r="P78" s="7">
         <f t="shared" ref="P78" si="23">(I78/H78)-1</f>
         <v>5.2497570075656697E-2</v>
       </c>
@@ -3649,22 +5338,22 @@
       <c r="K80" t="s">
         <v>41</v>
       </c>
-      <c r="L80" s="11">
+      <c r="L80" s="7">
         <v>0</v>
       </c>
-      <c r="M80" s="11">
+      <c r="M80" s="7">
         <f>(F80/E80)-1</f>
         <v>3.9103351715861434E-2</v>
       </c>
-      <c r="N80" s="11">
+      <c r="N80" s="7">
         <f t="shared" ref="N80:N82" si="25">(G80/F80)-1</f>
         <v>6.8615858437255151E-2</v>
       </c>
-      <c r="O80" s="11">
+      <c r="O80" s="7">
         <f t="shared" ref="O80:O82" si="26">(H80/G80)-1</f>
         <v>7.6150100036669333E-2</v>
       </c>
-      <c r="P80" s="11">
+      <c r="P80" s="7">
         <f t="shared" ref="P80:P82" si="27">(I80/H80)-1</f>
         <v>5.3897656623625112E-2</v>
       </c>
@@ -3696,22 +5385,22 @@
       <c r="K81" t="s">
         <v>42</v>
       </c>
-      <c r="L81" s="11">
+      <c r="L81" s="7">
         <v>0</v>
       </c>
-      <c r="M81" s="11">
+      <c r="M81" s="7">
         <f t="shared" ref="M81:M82" si="29">(F81/E81)-1</f>
         <v>3.5116668685156061E-2</v>
       </c>
-      <c r="N81" s="11">
+      <c r="N81" s="7">
         <f t="shared" si="25"/>
         <v>3.4573703120505783E-2</v>
       </c>
-      <c r="O81" s="11">
+      <c r="O81" s="7">
         <f t="shared" si="26"/>
         <v>3.241934039836214E-2</v>
       </c>
-      <c r="P81" s="11">
+      <c r="P81" s="7">
         <f t="shared" si="27"/>
         <v>3.2791112693348667E-2</v>
       </c>
@@ -3743,22 +5432,22 @@
       <c r="K82" t="s">
         <v>43</v>
       </c>
-      <c r="L82" s="11">
+      <c r="L82" s="7">
         <v>0</v>
       </c>
-      <c r="M82" s="11">
+      <c r="M82" s="7">
         <f t="shared" si="29"/>
         <v>6.6367956902914971E-2</v>
       </c>
-      <c r="N82" s="11">
+      <c r="N82" s="7">
         <f t="shared" si="25"/>
         <v>0.15334078158016173</v>
       </c>
-      <c r="O82" s="11">
+      <c r="O82" s="7">
         <f t="shared" si="26"/>
         <v>0.14280900887620684</v>
       </c>
-      <c r="P82" s="11">
+      <c r="P82" s="7">
         <f t="shared" si="27"/>
         <v>0.12990159946930047</v>
       </c>
@@ -3768,7 +5457,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P85"/>
   <sheetViews>
@@ -4386,22 +6075,22 @@
       <c r="I27">
         <v>1427892</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="7">
         <v>0</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="7">
         <f>(F27/E27)-1</f>
         <v>3.9106881696894913E-2</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="7">
         <f t="shared" ref="N27" si="0">(G27/F27)-1</f>
         <v>4.7421059980452096E-2</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="7">
         <f t="shared" ref="O27" si="1">(H27/G27)-1</f>
         <v>4.5192605801978925E-2</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P27" s="7">
         <f t="shared" ref="P27" si="2">(I27/H27)-1</f>
         <v>4.0672377678950156E-2</v>
       </c>
@@ -4439,22 +6128,22 @@
       <c r="K29" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="7">
         <v>0</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="7">
         <f>(F29/E29)-1</f>
         <v>3.2942024976980067E-2</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="7">
         <f t="shared" ref="N29:P31" si="4">(G29/F29)-1</f>
         <v>4.19615499335666E-2</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="7">
         <f t="shared" si="4"/>
         <v>4.2848034559483716E-2</v>
       </c>
-      <c r="P29" s="11">
+      <c r="P29" s="7">
         <f t="shared" si="4"/>
         <v>2.5291343298480262E-2</v>
       </c>
@@ -4486,22 +6175,22 @@
       <c r="K30" t="s">
         <v>42</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="7">
         <v>0</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="7">
         <f t="shared" ref="M30:M31" si="6">(F30/E30)-1</f>
         <v>3.3563071086480267E-2</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="7">
         <f t="shared" si="4"/>
         <v>2.7049700595856097E-2</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="7">
         <f t="shared" si="4"/>
         <v>2.4987484100615909E-2</v>
       </c>
-      <c r="P30" s="11">
+      <c r="P30" s="7">
         <f t="shared" si="4"/>
         <v>2.5517614492154062E-2</v>
       </c>
@@ -4533,22 +6222,22 @@
       <c r="K31" t="s">
         <v>43</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="7">
         <v>0</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="7">
         <f t="shared" si="6"/>
         <v>8.4793706711249195E-2</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="7">
         <f t="shared" si="4"/>
         <v>0.17244487254463525</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O31" s="7">
         <f t="shared" si="4"/>
         <v>0.14841939099460699</v>
       </c>
-      <c r="P31" s="11">
+      <c r="P31" s="7">
         <f t="shared" si="4"/>
         <v>0.13214035697313764</v>
       </c>
@@ -5099,22 +6788,22 @@
       <c r="I54">
         <v>705058</v>
       </c>
-      <c r="L54" s="11">
+      <c r="L54" s="7">
         <v>0</v>
       </c>
-      <c r="M54" s="11">
+      <c r="M54" s="7">
         <f>(F54/E54)-1</f>
         <v>4.0891917294819002E-2</v>
       </c>
-      <c r="N54" s="11">
+      <c r="N54" s="7">
         <f t="shared" ref="N54" si="8">(G54/F54)-1</f>
         <v>4.9043194065274243E-2</v>
       </c>
-      <c r="O54" s="11">
+      <c r="O54" s="7">
         <f t="shared" ref="O54" si="9">(H54/G54)-1</f>
         <v>4.6288340524435423E-2</v>
       </c>
-      <c r="P54" s="11">
+      <c r="P54" s="7">
         <f t="shared" ref="P54" si="10">(I54/H54)-1</f>
         <v>4.1369236200038628E-2</v>
       </c>
@@ -5152,22 +6841,22 @@
       <c r="K56" t="s">
         <v>41</v>
       </c>
-      <c r="L56" s="11">
+      <c r="L56" s="7">
         <v>0</v>
       </c>
-      <c r="M56" s="11">
+      <c r="M56" s="7">
         <f>(F56/E56)-1</f>
         <v>3.324750231743745E-2</v>
       </c>
-      <c r="N56" s="11">
+      <c r="N56" s="7">
         <f t="shared" ref="N56:N58" si="12">(G56/F56)-1</f>
         <v>4.2764010446779244E-2</v>
       </c>
-      <c r="O56" s="11">
+      <c r="O56" s="7">
         <f t="shared" ref="O56:O58" si="13">(H56/G56)-1</f>
         <v>4.359131232792901E-2</v>
       </c>
-      <c r="P56" s="11">
+      <c r="P56" s="7">
         <f t="shared" ref="P56:P58" si="14">(I56/H56)-1</f>
         <v>2.7388978455225033E-2</v>
       </c>
@@ -5199,22 +6888,22 @@
       <c r="K57" t="s">
         <v>42</v>
       </c>
-      <c r="L57" s="11">
+      <c r="L57" s="7">
         <v>0</v>
       </c>
-      <c r="M57" s="11">
+      <c r="M57" s="7">
         <f t="shared" ref="M57:M58" si="16">(F57/E57)-1</f>
         <v>3.3712357097277712E-2</v>
       </c>
-      <c r="N57" s="11">
+      <c r="N57" s="7">
         <f t="shared" si="12"/>
         <v>2.81752642748061E-2</v>
       </c>
-      <c r="O57" s="11">
+      <c r="O57" s="7">
         <f t="shared" si="13"/>
         <v>2.7391116694355233E-2</v>
       </c>
-      <c r="P57" s="11">
+      <c r="P57" s="7">
         <f t="shared" si="14"/>
         <v>2.7604302347140175E-2</v>
       </c>
@@ -5246,22 +6935,22 @@
       <c r="K58" t="s">
         <v>43</v>
       </c>
-      <c r="L58" s="11">
+      <c r="L58" s="7">
         <v>0</v>
       </c>
-      <c r="M58" s="11">
+      <c r="M58" s="7">
         <f t="shared" si="16"/>
         <v>0.10986029631978567</v>
       </c>
-      <c r="N58" s="11">
+      <c r="N58" s="7">
         <f t="shared" si="12"/>
         <v>0.19765393101477802</v>
       </c>
-      <c r="O58" s="11">
+      <c r="O58" s="7">
         <f t="shared" si="13"/>
         <v>0.15576996991424896</v>
       </c>
-      <c r="P58" s="11">
+      <c r="P58" s="7">
         <f t="shared" si="14"/>
         <v>0.13487913398467954</v>
       </c>
@@ -5812,22 +7501,22 @@
       <c r="I81">
         <v>722834</v>
       </c>
-      <c r="L81" s="11">
+      <c r="L81" s="7">
         <v>0</v>
       </c>
-      <c r="M81" s="11">
+      <c r="M81" s="7">
         <f>(F81/E81)-1</f>
         <v>3.7382751061454389E-2</v>
       </c>
-      <c r="N81" s="11">
+      <c r="N81" s="7">
         <f t="shared" ref="N81" si="18">(G81/F81)-1</f>
         <v>4.5848972710889946E-2</v>
       </c>
-      <c r="O81" s="11">
+      <c r="O81" s="7">
         <f t="shared" ref="O81" si="19">(H81/G81)-1</f>
         <v>4.4127433851663733E-2</v>
       </c>
-      <c r="P81" s="11">
+      <c r="P81" s="7">
         <f t="shared" ref="P81" si="20">(I81/H81)-1</f>
         <v>3.9993554299986966E-2</v>
       </c>
@@ -5865,22 +7554,22 @@
       <c r="K83" t="s">
         <v>41</v>
       </c>
-      <c r="L83" s="11">
+      <c r="L83" s="7">
         <v>0</v>
       </c>
-      <c r="M83" s="11">
+      <c r="M83" s="7">
         <f>(F83/E83)-1</f>
         <v>3.262422493356576E-2</v>
       </c>
-      <c r="N83" s="11">
+      <c r="N83" s="7">
         <f t="shared" ref="N83:N85" si="22">(G83/F83)-1</f>
         <v>4.1126214935491623E-2</v>
       </c>
-      <c r="O83" s="11">
+      <c r="O83" s="7">
         <f t="shared" ref="O83:O85" si="23">(H83/G83)-1</f>
         <v>4.2073089700996658E-2</v>
       </c>
-      <c r="P83" s="11">
+      <c r="P83" s="7">
         <f t="shared" ref="P83:P85" si="24">(I83/H83)-1</f>
         <v>2.310115282595393E-2</v>
       </c>
@@ -5912,22 +7601,22 @@
       <c r="K84" t="s">
         <v>42</v>
       </c>
-      <c r="L84" s="11">
+      <c r="L84" s="7">
         <v>0</v>
       </c>
-      <c r="M84" s="11">
+      <c r="M84" s="7">
         <f t="shared" ref="M84:M85" si="26">(F84/E84)-1</f>
         <v>3.3416091397198366E-2</v>
       </c>
-      <c r="N84" s="11">
+      <c r="N84" s="7">
         <f t="shared" si="22"/>
         <v>2.5941208066800225E-2</v>
       </c>
-      <c r="O84" s="11">
+      <c r="O84" s="7">
         <f t="shared" si="23"/>
         <v>2.2615152128127924E-2</v>
       </c>
-      <c r="P84" s="11">
+      <c r="P84" s="7">
         <f t="shared" si="24"/>
         <v>2.3448481294274348E-2</v>
       </c>
@@ -5959,22 +7648,22 @@
       <c r="K85" t="s">
         <v>43</v>
       </c>
-      <c r="L85" s="11">
+      <c r="L85" s="7">
         <v>0</v>
       </c>
-      <c r="M85" s="11">
+      <c r="M85" s="7">
         <f t="shared" si="26"/>
         <v>6.6367956902914971E-2</v>
       </c>
-      <c r="N85" s="11">
+      <c r="N85" s="7">
         <f t="shared" si="22"/>
         <v>0.153158623369684</v>
       </c>
-      <c r="O85" s="11">
+      <c r="O85" s="7">
         <f t="shared" si="23"/>
         <v>0.14257882432233204</v>
       </c>
-      <c r="P85" s="11">
+      <c r="P85" s="7">
         <f t="shared" si="24"/>
         <v>0.1299390766564974</v>
       </c>
@@ -5984,7 +7673,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P85"/>
   <sheetViews>
@@ -6602,22 +8291,22 @@
       <c r="I27">
         <v>1353185</v>
       </c>
-      <c r="L27" s="11">
+      <c r="L27" s="7">
         <v>0</v>
       </c>
-      <c r="M27" s="11">
+      <c r="M27" s="7">
         <f>(F27/E27)-1</f>
         <v>3.7490175400197057E-2</v>
       </c>
-      <c r="N27" s="11">
+      <c r="N27" s="7">
         <f t="shared" ref="N27" si="0">(G27/F27)-1</f>
         <v>3.4936769553491231E-2</v>
       </c>
-      <c r="O27" s="11">
+      <c r="O27" s="7">
         <f t="shared" ref="O27" si="1">(H27/G27)-1</f>
         <v>2.414187696028236E-2</v>
       </c>
-      <c r="P27" s="11">
+      <c r="P27" s="7">
         <f t="shared" ref="P27" si="2">(I27/H27)-1</f>
         <v>2.0224524261889698E-2</v>
       </c>
@@ -6655,22 +8344,22 @@
       <c r="K29" t="s">
         <v>41</v>
       </c>
-      <c r="L29" s="11">
+      <c r="L29" s="7">
         <v>0</v>
       </c>
-      <c r="M29" s="11">
+      <c r="M29" s="7">
         <f>(F29/E29)-1</f>
         <v>2.8989262069231136E-2</v>
       </c>
-      <c r="N29" s="11">
+      <c r="N29" s="7">
         <f t="shared" ref="N29:P31" si="4">(G29/F29)-1</f>
         <v>1.6774241841696069E-2</v>
       </c>
-      <c r="O29" s="11">
+      <c r="O29" s="7">
         <f t="shared" si="4"/>
         <v>3.1422232484363821E-3</v>
       </c>
-      <c r="P29" s="11">
+      <c r="P29" s="7">
         <f t="shared" si="4"/>
         <v>-1.2632934363449588E-2</v>
       </c>
@@ -6702,22 +8391,22 @@
       <c r="K30" t="s">
         <v>42</v>
       </c>
-      <c r="L30" s="11">
+      <c r="L30" s="7">
         <v>0</v>
       </c>
-      <c r="M30" s="11">
+      <c r="M30" s="7">
         <f t="shared" ref="M30:M31" si="6">(F30/E30)-1</f>
         <v>3.2543427046503037E-2</v>
       </c>
-      <c r="N30" s="11">
+      <c r="N30" s="7">
         <f t="shared" si="4"/>
         <v>1.7069590935619994E-2</v>
       </c>
-      <c r="O30" s="11">
+      <c r="O30" s="7">
         <f t="shared" si="4"/>
         <v>6.4321333060535224E-3</v>
       </c>
-      <c r="P30" s="11">
+      <c r="P30" s="7">
         <f t="shared" si="4"/>
         <v>6.1528505200150185E-3</v>
       </c>
@@ -6749,22 +8438,22 @@
       <c r="K31" t="s">
         <v>43</v>
       </c>
-      <c r="L31" s="11">
+      <c r="L31" s="7">
         <v>0</v>
       </c>
-      <c r="M31" s="11">
+      <c r="M31" s="7">
         <f t="shared" si="6"/>
         <v>8.4651898734177111E-2</v>
       </c>
-      <c r="N31" s="11">
+      <c r="N31" s="7">
         <f t="shared" si="4"/>
         <v>0.17151782888127376</v>
       </c>
-      <c r="O31" s="11">
+      <c r="O31" s="7">
         <f t="shared" si="4"/>
         <v>0.1469233841599511</v>
       </c>
-      <c r="P31" s="11">
+      <c r="P31" s="7">
         <f t="shared" si="4"/>
         <v>0.13057572746919588</v>
       </c>
@@ -7315,22 +9004,22 @@
       <c r="I54">
         <v>667645</v>
       </c>
-      <c r="L54" s="11">
+      <c r="L54" s="7">
         <v>0</v>
       </c>
-      <c r="M54" s="11">
+      <c r="M54" s="7">
         <f>(F54/E54)-1</f>
         <v>3.9241593558000165E-2</v>
       </c>
-      <c r="N54" s="11">
+      <c r="N54" s="7">
         <f t="shared" ref="N54" si="8">(G54/F54)-1</f>
         <v>3.6334202570039498E-2</v>
       </c>
-      <c r="O54" s="11">
+      <c r="O54" s="7">
         <f t="shared" ref="O54" si="9">(H54/G54)-1</f>
         <v>2.4898040401539756E-2</v>
       </c>
-      <c r="P54" s="11">
+      <c r="P54" s="7">
         <f t="shared" ref="P54" si="10">(I54/H54)-1</f>
         <v>2.065478938566101E-2</v>
       </c>
@@ -7368,22 +9057,22 @@
       <c r="K56" t="s">
         <v>41</v>
       </c>
-      <c r="L56" s="11">
+      <c r="L56" s="7">
         <v>0</v>
       </c>
-      <c r="M56" s="11">
+      <c r="M56" s="7">
         <f>(F56/E56)-1</f>
         <v>2.9313008548769171E-2</v>
       </c>
-      <c r="N56" s="11">
+      <c r="N56" s="7">
         <f t="shared" ref="N56:N58" si="12">(G56/F56)-1</f>
         <v>1.7697993382431498E-2</v>
       </c>
-      <c r="O56" s="11">
+      <c r="O56" s="7">
         <f t="shared" ref="O56:O58" si="13">(H56/G56)-1</f>
         <v>4.0312801116959562E-3</v>
       </c>
-      <c r="P56" s="11">
+      <c r="P56" s="7">
         <f t="shared" ref="P56:P58" si="14">(I56/H56)-1</f>
         <v>-1.0204214869558359E-2</v>
       </c>
@@ -7415,22 +9104,22 @@
       <c r="K57" t="s">
         <v>42</v>
       </c>
-      <c r="L57" s="11">
+      <c r="L57" s="7">
         <v>0</v>
       </c>
-      <c r="M57" s="11">
+      <c r="M57" s="7">
         <f t="shared" ref="M57:M58" si="16">(F57/E57)-1</f>
         <v>3.2705214844200414E-2</v>
       </c>
-      <c r="N57" s="11">
+      <c r="N57" s="7">
         <f t="shared" si="12"/>
         <v>1.8239344872510665E-2</v>
       </c>
-      <c r="O57" s="11">
+      <c r="O57" s="7">
         <f t="shared" si="13"/>
         <v>8.9587522086151949E-3</v>
       </c>
-      <c r="P57" s="11">
+      <c r="P57" s="7">
         <f t="shared" si="14"/>
         <v>8.446839500387604E-3</v>
       </c>
@@ -7462,22 +9151,22 @@
       <c r="K58" t="s">
         <v>43</v>
       </c>
-      <c r="L58" s="11">
+      <c r="L58" s="7">
         <v>0</v>
       </c>
-      <c r="M58" s="11">
+      <c r="M58" s="7">
         <f t="shared" si="16"/>
         <v>0.10964889100294206</v>
       </c>
-      <c r="N58" s="11">
+      <c r="N58" s="7">
         <f t="shared" si="12"/>
         <v>0.19645323638211054</v>
       </c>
-      <c r="O58" s="11">
+      <c r="O58" s="7">
         <f t="shared" si="13"/>
         <v>0.15392577062406287</v>
       </c>
-      <c r="P58" s="11">
+      <c r="P58" s="7">
         <f t="shared" si="14"/>
         <v>0.13312864387484047</v>
       </c>
@@ -8028,22 +9717,22 @@
       <c r="I81">
         <v>685540</v>
       </c>
-      <c r="L81" s="11">
+      <c r="L81" s="7">
         <v>0</v>
       </c>
-      <c r="M81" s="11">
+      <c r="M81" s="7">
         <f>(F81/E81)-1</f>
         <v>3.5798515186335145E-2</v>
       </c>
-      <c r="N81" s="11">
+      <c r="N81" s="7">
         <f t="shared" ref="N81" si="18">(G81/F81)-1</f>
         <v>3.3582529909096381E-2</v>
       </c>
-      <c r="O81" s="11">
+      <c r="O81" s="7">
         <f t="shared" ref="O81" si="19">(H81/G81)-1</f>
         <v>2.3407134951457742E-2</v>
       </c>
-      <c r="P81" s="11">
+      <c r="P81" s="7">
         <f t="shared" ref="P81" si="20">(I81/H81)-1</f>
         <v>1.9805839107680967E-2</v>
       </c>
@@ -8081,22 +9770,22 @@
       <c r="K83" t="s">
         <v>41</v>
       </c>
-      <c r="L83" s="11">
+      <c r="L83" s="7">
         <v>0</v>
       </c>
-      <c r="M83" s="11">
+      <c r="M83" s="7">
         <f>(F83/E83)-1</f>
         <v>2.8652455924793596E-2</v>
       </c>
-      <c r="N83" s="11">
+      <c r="N83" s="7">
         <f t="shared" ref="N83:N85" si="22">(G83/F83)-1</f>
         <v>1.5812609809790379E-2</v>
       </c>
-      <c r="O83" s="11">
+      <c r="O83" s="7">
         <f t="shared" ref="O83:O85" si="23">(H83/G83)-1</f>
         <v>2.2149908392354867E-3</v>
       </c>
-      <c r="P83" s="11">
+      <c r="P83" s="7">
         <f t="shared" ref="P83:P85" si="24">(I83/H83)-1</f>
         <v>-1.5170532060027275E-2</v>
       </c>
@@ -8128,22 +9817,22 @@
       <c r="K84" t="s">
         <v>42</v>
       </c>
-      <c r="L84" s="11">
+      <c r="L84" s="7">
         <v>0</v>
       </c>
-      <c r="M84" s="11">
+      <c r="M84" s="7">
         <f t="shared" ref="M84:M85" si="26">(F84/E84)-1</f>
         <v>3.2384138710588983E-2</v>
       </c>
-      <c r="N84" s="11">
+      <c r="N84" s="7">
         <f t="shared" si="22"/>
         <v>1.5917550364028754E-2</v>
       </c>
-      <c r="O84" s="11">
+      <c r="O84" s="7">
         <f t="shared" si="23"/>
         <v>3.9380875857621955E-3</v>
       </c>
-      <c r="P84" s="11">
+      <c r="P84" s="7">
         <f t="shared" si="24"/>
         <v>3.8771113842821503E-3</v>
       </c>
@@ -8175,22 +9864,22 @@
       <c r="K85" t="s">
         <v>43</v>
       </c>
-      <c r="L85" s="11">
+      <c r="L85" s="7">
         <v>0</v>
       </c>
-      <c r="M85" s="11">
+      <c r="M85" s="7">
         <f t="shared" si="26"/>
         <v>6.6277307986169598E-2</v>
       </c>
-      <c r="N85" s="11">
+      <c r="N85" s="7">
         <f t="shared" si="22"/>
         <v>0.15244294927069801</v>
       </c>
-      <c r="O85" s="11">
+      <c r="O85" s="7">
         <f t="shared" si="23"/>
         <v>0.14136219451792065</v>
       </c>
-      <c r="P85" s="11">
+      <c r="P85" s="7">
         <f t="shared" si="24"/>
         <v>0.12852592216425829</v>
       </c>

</xml_diff>